<commit_message>
Added the missing dot notation for Process ID
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zina/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{868BCFE3-13C8-B44A-994E-80677E74C8CB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A1D2A72B-7AFD-AA41-A5CF-F16E8019630E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27420" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19700" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="684">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2079,6 +2079,9 @@
   </si>
   <si>
     <t>sequencing_protocol.paired_end</t>
+  </si>
+  <si>
+    <t>process.process_core.process_id</t>
   </si>
 </sst>
 </file>
@@ -5460,8 +5463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5596,6 +5599,9 @@
       </c>
       <c r="J4" s="4" t="s">
         <v>461</v>
+      </c>
+      <c r="K4" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -5994,7 +6000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
hot fix to add developmental stage field, now required, to integration tests
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FF2097-11C8-BC47-9E72-52BE202135E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -19,13 +25,13 @@
     <sheet name="Dissociation protocol" sheetId="10" r:id="rId10"/>
     <sheet name="Enrichment protocol" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="692">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2105,12 +2111,18 @@
   </si>
   <si>
     <t>Project shortname</t>
+  </si>
+  <si>
+    <t>HsapDv:0000087</t>
+  </si>
+  <si>
+    <t>human adult stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2586,23 +2598,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="336">
+    <row r="1" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>689</v>
       </c>
@@ -2696,7 +2708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -2807,7 +2819,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1">
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -2869,16 +2881,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="238">
+    <row r="1" spans="1:17" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -2976,7 +2988,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>446</v>
       </c>
@@ -3055,7 +3067,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3076,7 +3088,7 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>453</v>
       </c>
@@ -3111,16 +3123,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="238">
+    <row r="1" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -3196,7 +3208,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -3216,7 +3228,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>447</v>
       </c>
@@ -3254,7 +3266,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3271,7 +3283,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>454</v>
       </c>
@@ -3319,16 +3331,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="126">
+    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -3360,7 +3372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -3392,7 +3404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3424,7 +3436,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>95</v>
       </c>
@@ -3456,7 +3468,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3471,7 +3483,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
@@ -3508,7 +3520,7 @@
     <mergeCell ref="A5:K5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3521,16 +3533,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:BC5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="31" max="31" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="309">
+    <row r="1" spans="1:55" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -3689,7 +3704,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="15">
+    <row r="2" spans="1:55" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -3856,7 +3871,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:55">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>199</v>
       </c>
@@ -3915,7 +3930,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>218</v>
       </c>
@@ -4082,7 +4097,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -4141,7 +4156,7 @@
       <c r="BB5" s="12"/>
       <c r="BC5" s="12"/>
     </row>
-    <row r="6" spans="1:55" s="4" customFormat="1" ht="15">
+    <row r="6" spans="1:55" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>249</v>
       </c>
@@ -4225,6 +4240,12 @@
       </c>
       <c r="AD6" s="4" t="s">
         <v>259</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>690</v>
       </c>
       <c r="AH6" s="4" t="s">
         <v>261</v>
@@ -4287,16 +4308,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="337">
+    <row r="1" spans="1:42" ht="395" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4424,7 +4445,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -4552,7 +4573,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>199</v>
       </c>
@@ -4617,7 +4638,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>340</v>
       </c>
@@ -4745,7 +4766,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -4791,7 +4812,7 @@
       <c r="AO5" s="12"/>
       <c r="AP5" s="12"/>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>366</v>
       </c>
@@ -4874,16 +4895,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" ht="294">
+    <row r="1" spans="1:33" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4981,7 +5002,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -5079,7 +5100,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>199</v>
       </c>
@@ -5134,7 +5155,7 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>426</v>
       </c>
@@ -5232,7 +5253,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
@@ -5269,7 +5290,7 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="4"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>448</v>
       </c>
@@ -5364,20 +5385,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="280">
+    <row r="1" spans="1:11" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>455</v>
       </c>
@@ -5412,7 +5433,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>463</v>
       </c>
@@ -5447,7 +5468,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>471</v>
       </c>
@@ -5466,7 +5487,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>476</v>
       </c>
@@ -5501,7 +5522,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
@@ -5516,7 +5537,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>686</v>
       </c>
@@ -5549,7 +5570,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>687</v>
       </c>
@@ -5582,7 +5603,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>688</v>
       </c>
@@ -5630,16 +5651,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="238">
+    <row r="1" spans="1:16" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -5686,7 +5707,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -5733,7 +5754,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -5762,7 +5783,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>365</v>
       </c>
@@ -5809,7 +5830,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -5829,7 +5850,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" ht="112">
+    <row r="6" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>374</v>
       </c>
@@ -5891,16 +5912,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="238">
+    <row r="1" spans="1:19" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -5954,7 +5975,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -6010,7 +6031,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -6036,7 +6057,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>484</v>
       </c>
@@ -6092,7 +6113,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6115,7 +6136,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>488</v>
       </c>
@@ -6172,16 +6193,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:47" ht="238">
+    <row r="1" spans="1:47" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -6321,7 +6342,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -6461,7 +6482,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -6550,7 +6571,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>483</v>
       </c>
@@ -6690,7 +6711,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6741,7 +6762,7 @@
       <c r="AT5" s="12"/>
       <c r="AU5" s="12"/>
     </row>
-    <row r="6" spans="1:47" s="4" customFormat="1">
+    <row r="6" spans="1:47" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>487</v>
       </c>

</xml_diff>

<commit_message>
hot fix added developmental stage fields, now required, to fix integration tests
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E9A13C-CB74-454D-BD3D-51338B06702C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -19,13 +25,13 @@
     <sheet name="Dissociation protocol" sheetId="10" r:id="rId10"/>
     <sheet name="Enrichment protocol" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="692">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2105,12 +2111,18 @@
   </si>
   <si>
     <t>Project shortname</t>
+  </si>
+  <si>
+    <t>HsapDv:0000087</t>
+  </si>
+  <si>
+    <t>human adult stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2586,23 +2598,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="336">
+    <row r="1" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>689</v>
       </c>
@@ -2696,7 +2708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -2807,7 +2819,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1">
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -2869,16 +2881,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="238">
+    <row r="1" spans="1:17" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -2976,7 +2988,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>446</v>
       </c>
@@ -3055,7 +3067,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3076,7 +3088,7 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>453</v>
       </c>
@@ -3111,16 +3123,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="238">
+    <row r="1" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -3196,7 +3208,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -3216,7 +3228,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>447</v>
       </c>
@@ -3254,7 +3266,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3271,7 +3283,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>454</v>
       </c>
@@ -3319,16 +3331,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="126">
+    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -3360,7 +3372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -3392,7 +3404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3424,7 +3436,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>95</v>
       </c>
@@ -3456,7 +3468,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3471,7 +3483,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
@@ -3508,7 +3520,7 @@
     <mergeCell ref="A5:K5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3521,16 +3533,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:BC5"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:55" ht="309">
+    <row r="1" spans="1:55" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -3689,7 +3701,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="15">
+    <row r="2" spans="1:55" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -3856,7 +3868,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:55">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>199</v>
       </c>
@@ -3915,7 +3927,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>218</v>
       </c>
@@ -4082,7 +4094,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -4141,7 +4153,7 @@
       <c r="BB5" s="12"/>
       <c r="BC5" s="12"/>
     </row>
-    <row r="6" spans="1:55" s="4" customFormat="1" ht="15">
+    <row r="6" spans="1:55" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>249</v>
       </c>
@@ -4225,6 +4237,12 @@
       </c>
       <c r="AD6" s="4" t="s">
         <v>259</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>690</v>
       </c>
       <c r="AH6" s="4" t="s">
         <v>261</v>
@@ -4287,16 +4305,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="337">
+    <row r="1" spans="1:42" ht="395" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4424,7 +4442,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -4552,7 +4570,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>199</v>
       </c>
@@ -4617,7 +4635,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>340</v>
       </c>
@@ -4745,7 +4763,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -4791,7 +4809,7 @@
       <c r="AO5" s="12"/>
       <c r="AP5" s="12"/>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>366</v>
       </c>
@@ -4874,16 +4892,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" ht="294">
+    <row r="1" spans="1:33" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4981,7 +4999,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -5079,7 +5097,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>199</v>
       </c>
@@ -5134,7 +5152,7 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>426</v>
       </c>
@@ -5232,7 +5250,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
@@ -5269,7 +5287,7 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="4"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>448</v>
       </c>
@@ -5364,20 +5382,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="280">
+    <row r="1" spans="1:11" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>455</v>
       </c>
@@ -5412,7 +5430,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>463</v>
       </c>
@@ -5447,7 +5465,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>471</v>
       </c>
@@ -5466,7 +5484,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>476</v>
       </c>
@@ -5501,7 +5519,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
@@ -5516,7 +5534,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>686</v>
       </c>
@@ -5549,7 +5567,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>687</v>
       </c>
@@ -5582,7 +5600,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>688</v>
       </c>
@@ -5630,16 +5648,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="238">
+    <row r="1" spans="1:16" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -5686,7 +5704,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -5733,7 +5751,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -5762,7 +5780,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>365</v>
       </c>
@@ -5809,7 +5827,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -5829,7 +5847,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" ht="112">
+    <row r="6" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>374</v>
       </c>
@@ -5891,16 +5909,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="238">
+    <row r="1" spans="1:19" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -5954,7 +5972,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -6010,7 +6028,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -6036,7 +6054,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>484</v>
       </c>
@@ -6092,7 +6110,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6115,7 +6133,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>488</v>
       </c>
@@ -6172,16 +6190,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:47" ht="238">
+    <row r="1" spans="1:47" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -6321,7 +6339,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -6461,7 +6479,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -6550,7 +6568,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>483</v>
       </c>
@@ -6690,7 +6708,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6741,7 +6759,7 @@
       <c r="AT5" s="12"/>
       <c r="AU5" s="12"/>
     </row>
-    <row r="6" spans="1:47" s="4" customFormat="1">
+    <row r="6" spans="1:47" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>487</v>
       </c>

</xml_diff>

<commit_message>
hot fix to keep up to date with int and staging added developmental stage field, now required, to integration sheets
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3C3352-8D9C-6B43-A3B5-9B0C01BF8F8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -19,13 +25,13 @@
     <sheet name="Dissociation protocol" sheetId="10" r:id="rId10"/>
     <sheet name="Enrichment protocol" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="692">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2105,12 +2111,18 @@
   </si>
   <si>
     <t>Project shortname</t>
+  </si>
+  <si>
+    <t>human adult stage</t>
+  </si>
+  <si>
+    <t>HsapDv:0000087</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2586,23 +2598,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="336">
+    <row r="1" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2649,7 +2661,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>689</v>
       </c>
@@ -2696,7 +2708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2740,7 +2752,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -2807,7 +2819,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1">
+    <row r="6" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>59</v>
       </c>
@@ -2869,16 +2881,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="238">
+    <row r="1" spans="1:17" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -2976,7 +2988,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>446</v>
       </c>
@@ -3055,7 +3067,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3076,7 +3088,7 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="12"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>453</v>
       </c>
@@ -3111,16 +3123,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="238">
+    <row r="1" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -3196,7 +3208,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -3216,7 +3228,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>447</v>
       </c>
@@ -3254,7 +3266,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3271,7 +3283,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>454</v>
       </c>
@@ -3319,16 +3331,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="126">
+    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -3360,7 +3372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>75</v>
       </c>
@@ -3392,7 +3404,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -3424,7 +3436,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>95</v>
       </c>
@@ -3456,7 +3468,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -3471,7 +3483,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>105</v>
       </c>
@@ -3508,7 +3520,7 @@
     <mergeCell ref="A5:K5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3521,16 +3533,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:BC5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:55" ht="309">
+    <row r="1" spans="1:55" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -3689,7 +3701,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="15">
+    <row r="2" spans="1:55" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -3856,7 +3868,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:55">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>199</v>
       </c>
@@ -3915,7 +3927,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>218</v>
       </c>
@@ -4082,7 +4094,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -4141,7 +4153,7 @@
       <c r="BB5" s="12"/>
       <c r="BC5" s="12"/>
     </row>
-    <row r="6" spans="1:55" s="4" customFormat="1" ht="15">
+    <row r="6" spans="1:55" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>249</v>
       </c>
@@ -4225,6 +4237,12 @@
       </c>
       <c r="AD6" s="4" t="s">
         <v>259</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>691</v>
       </c>
       <c r="AH6" s="4" t="s">
         <v>261</v>
@@ -4287,16 +4305,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:AP5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="337">
+    <row r="1" spans="1:42" ht="395" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4424,7 +4442,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -4552,7 +4570,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>199</v>
       </c>
@@ -4617,7 +4635,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>340</v>
       </c>
@@ -4745,7 +4763,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -4791,7 +4809,7 @@
       <c r="AO5" s="12"/>
       <c r="AP5" s="12"/>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>366</v>
       </c>
@@ -4874,16 +4892,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:33" ht="294">
+    <row r="1" spans="1:33" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
@@ -4981,7 +4999,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>147</v>
       </c>
@@ -5079,7 +5097,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>199</v>
       </c>
@@ -5134,7 +5152,7 @@
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>426</v>
       </c>
@@ -5232,7 +5250,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
@@ -5269,7 +5287,7 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="4"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>448</v>
       </c>
@@ -5364,20 +5382,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="280">
+    <row r="1" spans="1:11" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>455</v>
       </c>
@@ -5412,7 +5430,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>463</v>
       </c>
@@ -5447,7 +5465,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>471</v>
       </c>
@@ -5466,7 +5484,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>476</v>
       </c>
@@ -5501,7 +5519,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>58</v>
       </c>
@@ -5516,7 +5534,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>686</v>
       </c>
@@ -5549,7 +5567,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>687</v>
       </c>
@@ -5582,7 +5600,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>688</v>
       </c>
@@ -5630,16 +5648,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="238">
+    <row r="1" spans="1:16" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -5686,7 +5704,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -5733,7 +5751,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -5762,7 +5780,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>365</v>
       </c>
@@ -5809,7 +5827,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -5829,7 +5847,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" ht="112">
+    <row r="6" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>374</v>
       </c>
@@ -5891,16 +5909,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="238">
+    <row r="1" spans="1:19" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -5954,7 +5972,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -6010,7 +6028,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -6036,7 +6054,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>484</v>
       </c>
@@ -6092,7 +6110,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6115,7 +6133,7 @@
       <c r="R5" s="12"/>
       <c r="S5" s="12"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>488</v>
       </c>
@@ -6172,16 +6190,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AU6"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:47" ht="238">
+    <row r="1" spans="1:47" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -6321,7 +6339,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:47">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>412</v>
       </c>
@@ -6461,7 +6479,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:47">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>506</v>
       </c>
@@ -6550,7 +6568,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:47">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>483</v>
       </c>
@@ -6690,7 +6708,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="5" spans="1:47">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -6741,7 +6759,7 @@
       <c r="AT5" s="12"/>
       <c r="AU5" s="12"/>
     </row>
-    <row r="6" spans="1:47" s="4" customFormat="1">
+    <row r="6" spans="1:47" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>487</v>
       </c>

</xml_diff>

<commit_message>
hotfix to integration test 10x spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FF2097-11C8-BC47-9E72-52BE202135E3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540DF1FF-719F-8C49-B369-9FD88E21F767}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="687">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -478,9 +478,6 @@
     <t>The name of a mass unit being used.</t>
   </si>
   <si>
-    <t>Yes if entire body (but not limbs) was perfused with warm oxygenated blood. No otherwise.</t>
-  </si>
-  <si>
     <t>The biological sex of the organism.</t>
   </si>
   <si>
@@ -634,9 +631,6 @@
     <t>donor_organism.weight_unit.ontology_label</t>
   </si>
   <si>
-    <t>Normothermic regional perfusion?</t>
-  </si>
-  <si>
     <t>sex</t>
   </si>
   <si>
@@ -694,9 +688,6 @@
     <t>60</t>
   </si>
   <si>
-    <t>Should be one of: yes, no, or unknown.</t>
-  </si>
-  <si>
     <t>donor_organism.biomaterial_core.biomaterial_id</t>
   </si>
   <si>
@@ -784,9 +775,6 @@
     <t>donor_organism.weight</t>
   </si>
   <si>
-    <t>donor_organism.normothermic_regional_perfusion</t>
-  </si>
-  <si>
     <t>donor_organism.sex</t>
   </si>
   <si>
@@ -848,9 +836,6 @@
   </si>
   <si>
     <t>kilogram</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>male</t>
@@ -2352,7 +2337,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2404,7 +2389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2663,7 +2648,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2892,25 +2877,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>119</v>
@@ -2920,151 +2905,151 @@
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="K3" t="s">
+        <v>329</v>
+      </c>
+      <c r="L3" t="s">
+        <v>330</v>
+      </c>
+      <c r="M3" t="s">
+        <v>331</v>
+      </c>
+      <c r="N3" t="s">
+        <v>332</v>
+      </c>
+      <c r="O3" t="s">
+        <v>333</v>
+      </c>
+      <c r="P3" t="s">
         <v>334</v>
-      </c>
-      <c r="L3" t="s">
-        <v>335</v>
-      </c>
-      <c r="M3" t="s">
-        <v>336</v>
-      </c>
-      <c r="N3" t="s">
-        <v>337</v>
-      </c>
-      <c r="O3" t="s">
-        <v>338</v>
-      </c>
-      <c r="P3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>647</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>639</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>640</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>641</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>648</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>649</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>650</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>651</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>653</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -3090,22 +3075,22 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -3134,25 +3119,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>119</v>
@@ -3161,109 +3146,109 @@
         <v>120</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>662</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="J3" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="K3" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
       <c r="L3" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>673</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>674</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>675</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>662</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>663</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>664</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>676</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>677</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3285,29 +3270,29 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
       <c r="K6" s="4">
         <v>70</v>
@@ -3536,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3700,401 +3685,390 @@
       <c r="BB1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BC1" s="1"/>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="2" spans="1:55" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="AK2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="AH2" s="2" t="s">
-        <v>680</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AO2" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AR2" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AS2" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AV2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AW2" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AY2" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="AY2" s="2" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="BC2" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" t="s">
         <v>199</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>200</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>201</v>
       </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>202</v>
       </c>
-      <c r="H3" t="s">
+      <c r="N3" t="s">
         <v>203</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>204</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>205</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>206</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>207</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>208</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>209</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AA3" t="s">
         <v>210</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AN3" t="s">
         <v>211</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AR3" t="s">
         <v>212</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AV3" t="s">
         <v>213</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AX3" t="s">
         <v>214</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>215</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>216</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="L4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="X4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA4" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="AB4" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="AK4" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="X4" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AM4" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="AB4" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>680</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>681</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>684</v>
-      </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AN4" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="AP4" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR4" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AS4" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AV4" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AW4" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="AO4" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="AQ4" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AX4" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="AS4" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="AV4" s="4" t="s">
+      <c r="AY4" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="BA4" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="BB4" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="AX4" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="BA4" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="BB4" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="BC4" s="4" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:55" x14ac:dyDescent="0.2">
@@ -4154,44 +4128,43 @@
       <c r="AZ5" s="12"/>
       <c r="BA5" s="12"/>
       <c r="BB5" s="12"/>
-      <c r="BC5" s="12"/>
     </row>
     <row r="6" spans="1:55" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D6" s="4">
         <v>9606</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="H6" s="4">
         <v>36.4</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>109</v>
@@ -4203,73 +4176,73 @@
         <v>0</v>
       </c>
       <c r="P6" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="R6" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="Q6" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>208</v>
-      </c>
       <c r="S6" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="T6" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="U6" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="X6" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AA6" s="4">
         <v>20</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="AE6" s="4" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AI6" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AN6" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AR6" s="4">
         <v>160</v>
       </c>
       <c r="AS6" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AT6" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AU6" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="AV6" s="4" t="s">
         <v>109</v>
@@ -4278,24 +4251,21 @@
         <v>60</v>
       </c>
       <c r="AY6" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AZ6" s="4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="BA6" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="BB6" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="BC6" s="4" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:BC5"/>
+    <mergeCell ref="A5:BB5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4355,7 +4325,7 @@
         <v>137</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>120</v>
@@ -4364,7 +4334,7 @@
         <v>137</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>120</v>
@@ -4379,34 +4349,34 @@
         <v>120</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>135</v>
@@ -4418,352 +4388,352 @@
         <v>120</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AP1" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="AP1" s="5" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="R2" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="W2" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>682</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AE2" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AM2" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AN2" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
         <v>199</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>200</v>
       </c>
-      <c r="G3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H3" t="s">
-        <v>202</v>
-      </c>
       <c r="U3" t="s">
+        <v>318</v>
+      </c>
+      <c r="W3" t="s">
+        <v>319</v>
+      </c>
+      <c r="X3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>321</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>322</v>
+      </c>
+      <c r="AA3" t="s">
         <v>323</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AB3" t="s">
         <v>324</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AC3" t="s">
         <v>325</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AD3" t="s">
         <v>326</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AH3" t="s">
         <v>327</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AI3" t="s">
         <v>328</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AJ3" t="s">
         <v>329</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AK3" t="s">
         <v>330</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AL3" t="s">
         <v>331</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AM3" t="s">
         <v>332</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AN3" t="s">
         <v>333</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AO3" t="s">
         <v>334</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>335</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>336</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>337</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>338</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="I4" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>682</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>683</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>685</v>
-      </c>
-      <c r="U4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="AB4" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="AC4" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>351</v>
       </c>
-      <c r="Z4" s="4" t="s">
+      <c r="AE4" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="AH4" s="4" t="s">
         <v>352</v>
       </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="AE4" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AM4" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AN4" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AP4" s="4" t="s">
         <v>360</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="AN4" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="AO4" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.2">
@@ -4814,70 +4784,70 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="I6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="R6" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="S6" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="U6" t="s">
+        <v>367</v>
+      </c>
+      <c r="V6" t="s">
         <v>368</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="AP6" s="4" t="s">
         <v>369</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="U6" t="s">
-        <v>372</v>
-      </c>
-      <c r="V6" t="s">
-        <v>373</v>
-      </c>
-      <c r="AP6" s="4" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -4930,10 +4900,10 @@
         <v>116</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>141</v>
@@ -4945,34 +4915,34 @@
         <v>120</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>133</v>
@@ -4984,7 +4954,7 @@
         <v>120</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>119</v>
@@ -4993,264 +4963,264 @@
         <v>120</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="AE1" s="8" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="AF1" s="8" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="I2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="P2" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AC2" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>412</v>
-      </c>
       <c r="AF2" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" t="s">
         <v>199</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>200</v>
       </c>
-      <c r="G3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H3" t="s">
-        <v>202</v>
-      </c>
       <c r="I3" t="s">
+        <v>408</v>
+      </c>
+      <c r="J3" t="s">
+        <v>409</v>
+      </c>
+      <c r="N3" t="s">
+        <v>410</v>
+      </c>
+      <c r="O3" t="s">
+        <v>411</v>
+      </c>
+      <c r="P3" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q3" t="s">
         <v>413</v>
       </c>
-      <c r="J3" t="s">
+      <c r="R3" t="s">
         <v>414</v>
       </c>
-      <c r="N3" t="s">
+      <c r="S3" t="s">
         <v>415</v>
       </c>
-      <c r="O3" t="s">
+      <c r="T3" t="s">
         <v>416</v>
       </c>
-      <c r="P3" t="s">
+      <c r="U3" t="s">
         <v>417</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="V3" t="s">
         <v>418</v>
       </c>
-      <c r="R3" t="s">
+      <c r="W3" t="s">
         <v>419</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AD3" t="s">
         <v>420</v>
-      </c>
-      <c r="T3" t="s">
-        <v>421</v>
-      </c>
-      <c r="U3" t="s">
-        <v>422</v>
-      </c>
-      <c r="V3" t="s">
-        <v>423</v>
-      </c>
-      <c r="W3" t="s">
-        <v>424</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>425</v>
       </c>
       <c r="AF3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="K4" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>431</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>432</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>392</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>435</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>436</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="X4" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="AD4" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="AE4" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="AF4" s="4" t="s">
         <v>442</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>443</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -5292,46 +5262,46 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E6" s="4">
         <v>9606</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>202</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="K6" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="N6" s="4">
         <v>85.3</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="P6" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="Q6" s="4">
         <v>10</v>
@@ -5340,34 +5310,34 @@
         <v>22</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AD6" s="10">
         <v>10000</v>
       </c>
       <c r="AE6" s="4" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="AF6" s="4" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -5400,126 +5370,126 @@
   <sheetData>
     <row r="1" spans="1:11" ht="365" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="I2" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="E3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="F3" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="G3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H3" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>479</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="K4" t="s">
         <v>480</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>481</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>482</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>483</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="K4" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -5539,101 +5509,101 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -5662,25 +5632,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>498</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>119</v>
@@ -5689,145 +5659,145 @@
         <v>120</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="J3" t="s">
+        <v>329</v>
+      </c>
+      <c r="K3" t="s">
+        <v>330</v>
+      </c>
+      <c r="L3" t="s">
+        <v>331</v>
+      </c>
+      <c r="M3" t="s">
+        <v>332</v>
+      </c>
+      <c r="N3" t="s">
+        <v>333</v>
+      </c>
+      <c r="O3" t="s">
         <v>334</v>
-      </c>
-      <c r="K3" t="s">
-        <v>335</v>
-      </c>
-      <c r="L3" t="s">
-        <v>336</v>
-      </c>
-      <c r="M3" t="s">
-        <v>337</v>
-      </c>
-      <c r="N3" t="s">
-        <v>338</v>
-      </c>
-      <c r="O3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>503</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="J4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>514</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>515</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -5852,49 +5822,49 @@
     </row>
     <row r="6" spans="1:16" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="J6" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>334</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -5923,25 +5893,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>497</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>119</v>
@@ -5950,11 +5920,11 @@
         <v>120</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>119</v>
@@ -5963,95 +5933,95 @@
         <v>120</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>539</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="J3" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="O3" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="P3" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="Q3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R3" t="s">
         <v>92</v>
@@ -6059,58 +6029,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>544</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="K4" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="O4" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>529</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>530</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>549</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>534</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>536</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>550</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>551</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>552</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -6138,38 +6108,38 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C6" s="4"/>
       <c r="G6" s="4" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>109</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="Q6" s="4">
         <v>4</v>
@@ -6204,34 +6174,34 @@
   <sheetData>
     <row r="1" spans="1:47" ht="288" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>497</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>119</v>
@@ -6240,7 +6210,7 @@
         <v>120</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>119</v>
@@ -6249,82 +6219,82 @@
         <v>120</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="V1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>290</v>
-      </c>
       <c r="AK1" s="1" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>119</v>
@@ -6333,7 +6303,7 @@
         <v>120</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>119</v>
@@ -6344,371 +6314,371 @@
     </row>
     <row r="2" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="N2" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="O2" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="P2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="AK2" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="AL2" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AP2" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="AE2" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AT2" s="3" t="s">
         <v>582</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E3" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G3" t="s">
+        <v>583</v>
+      </c>
+      <c r="I3" t="s">
+        <v>584</v>
+      </c>
+      <c r="P3" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>330</v>
+      </c>
+      <c r="R3" t="s">
+        <v>331</v>
+      </c>
+      <c r="S3" t="s">
+        <v>332</v>
+      </c>
+      <c r="T3" t="s">
+        <v>333</v>
+      </c>
+      <c r="U3" t="s">
+        <v>334</v>
+      </c>
+      <c r="V3" t="s">
+        <v>329</v>
+      </c>
+      <c r="W3" t="s">
+        <v>330</v>
+      </c>
+      <c r="X3" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>334</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>585</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>586</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>587</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>329</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>330</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>331</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>333</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>334</v>
+      </c>
+      <c r="AK3" t="s">
         <v>588</v>
       </c>
-      <c r="I3" t="s">
-        <v>589</v>
-      </c>
-      <c r="P3" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>335</v>
-      </c>
-      <c r="R3" t="s">
-        <v>336</v>
-      </c>
-      <c r="S3" t="s">
-        <v>337</v>
-      </c>
-      <c r="T3" t="s">
-        <v>338</v>
-      </c>
-      <c r="U3" t="s">
-        <v>339</v>
-      </c>
-      <c r="V3" t="s">
-        <v>334</v>
-      </c>
-      <c r="W3" t="s">
-        <v>335</v>
-      </c>
-      <c r="X3" t="s">
-        <v>336</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>337</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>338</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>339</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>590</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>591</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>592</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>334</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>335</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>336</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>337</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>338</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>339</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>593</v>
-      </c>
       <c r="AL3" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="AN3" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>594</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>595</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="J4" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>600</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>601</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="O4" s="4" t="s">
+      <c r="U4" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="AC4" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="AD4" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE4" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="AF4" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="AJ4" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="AK4" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="AL4" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="AM4" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="AO4" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>605</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>608</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>610</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>611</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>612</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>613</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>614</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>616</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>619</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>620</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>621</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>623</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>624</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>625</v>
-      </c>
-      <c r="AN4" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AP4" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="AR4" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="AS4" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="AT4" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>583</v>
-      </c>
-      <c r="AQ4" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="AR4" s="4" t="s">
-        <v>585</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>586</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -6764,50 +6734,50 @@
     </row>
     <row r="6" spans="1:47" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="K6" t="s">
+        <v>624</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="M6" t="s">
+        <v>625</v>
+      </c>
+      <c r="N6" t="s">
+        <v>626</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>628</v>
-      </c>
-      <c r="K6" t="s">
-        <v>629</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>628</v>
-      </c>
-      <c r="M6" t="s">
-        <v>630</v>
-      </c>
-      <c r="N6" t="s">
-        <v>631</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>632</v>
       </c>
       <c r="P6"/>
       <c r="AB6" s="11" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="AD6" s="4" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="AL6" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="AM6" s="4">
         <v>0</v>
@@ -6816,13 +6786,13 @@
         <v>16</v>
       </c>
       <c r="AO6" s="4" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="AQ6" s="4" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add reference to new 10x files.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D551D7-B6D3-CD44-AF41-8EF330C1EBBD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869A67BD-C5C6-DE43-91FF-CF5D466A32C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="2440" windowWidth="28660" windowHeight="18860" tabRatio="993" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19500" yWindow="2440" windowWidth="28660" windowHeight="18860" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="700">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2029,15 +2029,6 @@
     <t>specimen_from_organism.diseases.ontology_label</t>
   </si>
   <si>
-    <t>pbmc4k_S1_L001_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>pbmc4k_S1_L001_R2_001.fastq.gz</t>
-  </si>
-  <si>
-    <t>pbmc4k_S1_L001_I1_001.fastq.gz</t>
-  </si>
-  <si>
     <t>Project shortname</t>
   </si>
   <si>
@@ -2132,13 +2123,31 @@
   </si>
   <si>
     <t>Contains a small file set from the dataset: 4k PBMCs from a Healthy Donor, a Single Cell Gene Expression Dataset by Cell Ranger 2.1.0. Peripheral blood mononuclear cells (PBMCs) were taken from a healthy donor (same donor as pbmc8k). PBMCs are primary cells with relatively small amounts of RNA (~1pg RNA/cell). Data/Analysis can be found here https://support.10xgenomics.com/single-cell-gene-expression/datasets/2.1.0/pbmc4k and all data is licensed under the creative commons attribution license (https://creativecommons.org/licenses/by/4.0/). This test also contains extensive metadata for browser testing. Metadata is fabricated.</t>
+  </si>
+  <si>
+    <t>pbmc4k_1000_S1_L001_I1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>pbmc4k_1000_S1_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>pbmc4k_1000_S1_L001_R2_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3d252f83492bf030ddfd05a5a1411cdc</t>
+  </si>
+  <si>
+    <t>eeaf6532a43b731e1ed9068bf32add47</t>
+  </si>
+  <si>
+    <t>891e3067ff772d599a5c424f5a93bfd5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2176,22 +2185,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2202,12 +2197,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD0D0D0"/>
         <bgColor rgb="FFC0C0C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2223,7 +2212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2251,12 +2240,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2643,7 +2626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -2703,7 +2686,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2861,13 +2844,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>59</v>
@@ -3489,13 +3472,13 @@
     </row>
     <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>487</v>
@@ -3791,13 +3774,13 @@
     </row>
     <row r="6" spans="1:19" s="8" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>487</v>
@@ -4670,13 +4653,13 @@
     </row>
     <row r="6" spans="1:55" s="8" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D6" s="8">
         <v>9606</v>
@@ -4715,13 +4698,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>245</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="S6" s="8" t="s">
         <v>204</v>
@@ -4730,7 +4713,7 @@
         <v>246</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="X6" s="8" t="s">
         <v>247</v>
@@ -4754,10 +4737,10 @@
         <v>249</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="AH6" s="8" t="s">
         <v>251</v>
@@ -5320,16 +5303,16 @@
     </row>
     <row r="6" spans="1:42" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="E6" s="10">
         <v>9606</v>
@@ -5386,7 +5369,7 @@
         <v>360</v>
       </c>
       <c r="AP6" s="8" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>
@@ -5798,16 +5781,16 @@
     </row>
     <row r="6" spans="1:33" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5876,10 +5859,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="AF6" s="8" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -5900,14 +5883,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="33.5" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
@@ -6053,101 +6037,107 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>662</v>
+      <c r="A6" s="8" t="s">
+        <v>695</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>677</v>
-      </c>
-      <c r="C6" s="11" t="s">
+        <v>674</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="8" t="s">
+        <v>698</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="8">
         <v>26</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="8" t="s">
         <v>458</v>
       </c>
       <c r="I6" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>686</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>689</v>
-      </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="8" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>663</v>
+      <c r="A7" s="8" t="s">
+        <v>696</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>677</v>
-      </c>
-      <c r="C7" s="11" t="s">
+        <v>674</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="8" t="s">
+        <v>699</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="8">
         <v>98</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="8" t="s">
         <v>458</v>
       </c>
       <c r="I7" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="J7" s="8" t="s">
         <v>686</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>689</v>
-      </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="8" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
-        <v>664</v>
+      <c r="A8" s="8" t="s">
+        <v>694</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>677</v>
-      </c>
-      <c r="C8" s="11" t="s">
+        <v>674</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="8" t="s">
+        <v>697</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="8">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="8">
         <v>8</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="8" t="s">
         <v>458</v>
       </c>
       <c r="I8" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>686</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>689</v>
-      </c>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="8" t="s">
         <v>470</v>
       </c>
     </row>
@@ -6370,13 +6360,13 @@
     </row>
     <row r="6" spans="1:16" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>487</v>
@@ -6636,13 +6626,13 @@
     </row>
     <row r="6" spans="1:17" s="8" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>487</v>
@@ -6842,13 +6832,13 @@
     </row>
     <row r="6" spans="1:13" s="8" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>487</v>

</xml_diff>

<commit_message>
changed 10x integration test disease metadata
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FEA5A7-F14E-414F-88B4-D38DA5582700}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B805B65-8608-B047-BBD9-5D6C495088C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18280" yWindow="460" windowWidth="32920" windowHeight="20840" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8620" yWindow="9020" windowWidth="34240" windowHeight="18860" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -788,12 +788,6 @@
     <t>UO:0000036</t>
   </si>
   <si>
-    <t>atrophic vulva</t>
-  </si>
-  <si>
-    <t>MONDO:0001932</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
@@ -2154,6 +2148,12 @@
   </si>
   <si>
     <t>FILL OUT INFORMATION BELOW THIS ROW</t>
+  </si>
+  <si>
+    <t>H syndrome</t>
+  </si>
+  <si>
+    <t>MONDO:0011273</t>
   </si>
 </sst>
 </file>
@@ -2282,15 +2282,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2727,7 +2727,7 @@
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2855,13 +2855,13 @@
     </row>
     <row r="6" spans="1:13" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>56</v>
@@ -2919,25 +2919,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>476</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>
@@ -2946,109 +2946,109 @@
         <v>114</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>639</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F3" t="s">
         <v>484</v>
       </c>
-      <c r="E3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F3" t="s">
-        <v>486</v>
-      </c>
       <c r="J3" t="s">
+        <v>640</v>
+      </c>
+      <c r="K3" t="s">
+        <v>641</v>
+      </c>
+      <c r="L3" t="s">
         <v>642</v>
-      </c>
-      <c r="K3" t="s">
-        <v>643</v>
-      </c>
-      <c r="L3" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>650</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3070,34 +3070,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>687</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>688</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>486</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>
@@ -3129,34 +3129,34 @@
   <sheetData>
     <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>539</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>113</v>
@@ -3165,7 +3165,7 @@
         <v>114</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>113</v>
@@ -3174,82 +3174,82 @@
         <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="V1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="AB1" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>545</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>113</v>
@@ -3258,7 +3258,7 @@
         <v>114</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>113</v>
@@ -3269,371 +3269,371 @@
     </row>
     <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>562</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F3" t="s">
         <v>484</v>
       </c>
-      <c r="E3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F3" t="s">
-        <v>486</v>
-      </c>
       <c r="G3" t="s">
+        <v>563</v>
+      </c>
+      <c r="I3" t="s">
+        <v>564</v>
+      </c>
+      <c r="P3" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>319</v>
+      </c>
+      <c r="R3" t="s">
+        <v>320</v>
+      </c>
+      <c r="S3" t="s">
+        <v>321</v>
+      </c>
+      <c r="T3" t="s">
+        <v>322</v>
+      </c>
+      <c r="U3" t="s">
+        <v>323</v>
+      </c>
+      <c r="V3" t="s">
+        <v>318</v>
+      </c>
+      <c r="W3" t="s">
+        <v>319</v>
+      </c>
+      <c r="X3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>321</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>322</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB3" t="s">
         <v>565</v>
       </c>
-      <c r="I3" t="s">
+      <c r="AC3" t="s">
         <v>566</v>
       </c>
-      <c r="P3" t="s">
+      <c r="AD3" t="s">
+        <v>567</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>318</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AG3" t="s">
         <v>320</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="AH3" t="s">
         <v>321</v>
       </c>
-      <c r="R3" t="s">
+      <c r="AI3" t="s">
         <v>322</v>
       </c>
-      <c r="S3" t="s">
+      <c r="AJ3" t="s">
         <v>323</v>
       </c>
-      <c r="T3" t="s">
-        <v>324</v>
-      </c>
-      <c r="U3" t="s">
-        <v>325</v>
-      </c>
-      <c r="V3" t="s">
-        <v>320</v>
-      </c>
-      <c r="W3" t="s">
-        <v>321</v>
-      </c>
-      <c r="X3" t="s">
-        <v>322</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>323</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>324</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>325</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>567</v>
-      </c>
-      <c r="AC3" t="s">
+      <c r="AK3" t="s">
         <v>568</v>
       </c>
-      <c r="AD3" t="s">
-        <v>569</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>320</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>321</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>322</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>323</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>324</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>325</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>570</v>
-      </c>
       <c r="AL3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="AN3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>599</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>600</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="AM4" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>603</v>
-      </c>
       <c r="AO4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>562</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -3689,53 +3689,53 @@
     </row>
     <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>681</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>682</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>486</v>
-      </c>
       <c r="J6" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>604</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>605</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>604</v>
-      </c>
-      <c r="M6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>606</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>608</v>
       </c>
       <c r="P6" s="7"/>
       <c r="AB6" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>609</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AL6" s="7" t="s">
         <v>610</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>611</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>612</v>
       </c>
       <c r="AM6" s="6">
         <v>0</v>
@@ -3744,13 +3744,13 @@
         <v>16</v>
       </c>
       <c r="AO6" s="6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -3776,25 +3776,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>475</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>
@@ -3803,11 +3803,11 @@
         <v>114</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>113</v>
@@ -3816,92 +3816,92 @@
         <v>114</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>504</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F3" t="s">
         <v>484</v>
       </c>
-      <c r="E3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F3" t="s">
-        <v>486</v>
-      </c>
       <c r="J3" t="s">
+        <v>517</v>
+      </c>
+      <c r="O3" t="s">
+        <v>518</v>
+      </c>
+      <c r="P3" t="s">
         <v>519</v>
-      </c>
-      <c r="O3" t="s">
-        <v>520</v>
-      </c>
-      <c r="P3" t="s">
-        <v>521</v>
       </c>
       <c r="Q3" t="s">
         <v>197</v>
@@ -3912,58 +3912,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>514</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3991,49 +3991,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>684</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>685</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>486</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>103</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -4260,75 +4260,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CEF08FF-926B-F94C-BBDA-A05F5291FA20}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="25.6640625" style="14" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="14"/>
+    <col min="1" max="3" width="25.6640625" style="13" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
+        <v>695</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>696</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>697</v>
       </c>
-      <c r="B1" s="13" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
         <v>698</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>700</v>
       </c>
-      <c r="B3" s="15" t="s">
+    </row>
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
         <v>701</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>703</v>
-      </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4341,8 +4341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6:AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4608,13 +4608,13 @@
         <v>172</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>173</v>
@@ -4828,13 +4828,13 @@
         <v>172</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>230</v>
@@ -4951,13 +4951,13 @@
     </row>
     <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>662</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>664</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4996,13 +4996,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>242</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>201</v>
@@ -5011,7 +5011,7 @@
         <v>243</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>244</v>
@@ -5035,19 +5035,19 @@
         <v>246</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>660</v>
-      </c>
-      <c r="AH6" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="AI6" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="AJ6" s="7" t="s">
-        <v>248</v>
+        <v>658</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>702</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>703</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>702</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>205</v>
@@ -5056,13 +5056,13 @@
         <v>160</v>
       </c>
       <c r="AS6" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="AT6" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="AU6" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="AT6" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="AU6" s="7" t="s">
-        <v>252</v>
       </c>
       <c r="AV6" s="7" t="s">
         <v>103</v>
@@ -5071,16 +5071,16 @@
         <v>60</v>
       </c>
       <c r="AY6" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AZ6" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="BA6" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="AZ6" s="7" t="s">
+      <c r="BB6" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="BA6" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="BB6" s="7" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -5099,7 +5099,7 @@
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:AP5"/>
+      <selection activeCell="R6" sqref="R6:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5142,7 +5142,7 @@
         <v>131</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>114</v>
@@ -5151,7 +5151,7 @@
         <v>131</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>114</v>
@@ -5166,34 +5166,34 @@
         <v>114</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>129</v>
@@ -5205,31 +5205,31 @@
         <v>114</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>275</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5258,106 +5258,106 @@
         <v>146</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
@@ -5374,183 +5374,183 @@
         <v>194</v>
       </c>
       <c r="U3" t="s">
+        <v>307</v>
+      </c>
+      <c r="W3" t="s">
+        <v>308</v>
+      </c>
+      <c r="X3" t="s">
         <v>309</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>310</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>311</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>312</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>313</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>314</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>315</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AH3" t="s">
         <v>316</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AI3" t="s">
         <v>317</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AJ3" t="s">
         <v>318</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AK3" t="s">
         <v>319</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
         <v>320</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AM3" t="s">
         <v>321</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AN3" t="s">
         <v>322</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AO3" t="s">
         <v>323</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>324</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>658</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="AH4" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="AE4" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.2">
@@ -5601,16 +5601,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>668</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>662</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>669</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>670</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5634,40 +5634,40 @@
         <v>244</v>
       </c>
       <c r="L6" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="Q6" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="R6" t="s">
+        <v>702</v>
+      </c>
+      <c r="S6" t="s">
+        <v>703</v>
+      </c>
+      <c r="T6" t="s">
+        <v>702</v>
+      </c>
+      <c r="U6" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="V6" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="Q6" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>357</v>
-      </c>
       <c r="AP6" s="7" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
   </sheetData>
@@ -5685,7 +5685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -5717,10 +5717,10 @@
         <v>110</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>135</v>
@@ -5732,34 +5732,34 @@
         <v>114</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>127</v>
@@ -5771,7 +5771,7 @@
         <v>114</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>113</v>
@@ -5780,13 +5780,13 @@
         <v>114</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5815,76 +5815,76 @@
         <v>146</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>395</v>
-      </c>
       <c r="AF2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -5901,143 +5901,143 @@
         <v>194</v>
       </c>
       <c r="I3" t="s">
+        <v>394</v>
+      </c>
+      <c r="J3" t="s">
+        <v>395</v>
+      </c>
+      <c r="N3" t="s">
         <v>396</v>
       </c>
-      <c r="J3" t="s">
+      <c r="O3" t="s">
         <v>397</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>398</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>399</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>400</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>401</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>402</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>403</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>404</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>405</v>
       </c>
-      <c r="V3" t="s">
+      <c r="AD3" t="s">
         <v>406</v>
-      </c>
-      <c r="W3" t="s">
-        <v>407</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>408</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="AD4" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="X4" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>428</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -6073,22 +6073,22 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
       <c r="AG5" s="3"/>
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>671</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>668</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>672</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>673</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -6103,28 +6103,28 @@
         <v>194</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>430</v>
+      </c>
+      <c r="M6" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>433</v>
       </c>
       <c r="N6" s="6">
         <v>85.3</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="Q6" s="6">
         <v>10</v>
@@ -6133,16 +6133,16 @@
         <v>22</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>244</v>
@@ -6157,10 +6157,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
   </sheetData>
@@ -6197,126 +6197,126 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
+        <v>449</v>
+      </c>
+      <c r="E3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F3" t="s">
         <v>451</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>452</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>453</v>
-      </c>
-      <c r="G3" t="s">
-        <v>454</v>
-      </c>
-      <c r="H3" t="s">
-        <v>455</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" t="s">
         <v>463</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="K4" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6331,24 +6331,24 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6357,33 +6357,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6392,33 +6392,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6427,16 +6427,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -6468,25 +6468,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>476</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>
@@ -6495,145 +6495,145 @@
         <v>114</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>483</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F3" t="s">
         <v>484</v>
       </c>
-      <c r="E3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F3" t="s">
-        <v>486</v>
-      </c>
       <c r="J3" t="s">
+        <v>318</v>
+      </c>
+      <c r="K3" t="s">
+        <v>319</v>
+      </c>
+      <c r="L3" t="s">
         <v>320</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>321</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>322</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>323</v>
-      </c>
-      <c r="N3" t="s">
-        <v>324</v>
-      </c>
-      <c r="O3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>493</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6658,49 +6658,49 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>675</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>676</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>486</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>320</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -6726,25 +6726,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>474</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>476</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>113</v>
@@ -6754,151 +6754,151 @@
       </c>
       <c r="J1" s="1"/>
       <c r="K1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>616</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>618</v>
-      </c>
       <c r="K2" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F3" t="s">
         <v>484</v>
       </c>
-      <c r="E3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F3" t="s">
-        <v>486</v>
-      </c>
       <c r="K3" t="s">
+        <v>318</v>
+      </c>
+      <c r="L3" t="s">
+        <v>319</v>
+      </c>
+      <c r="M3" t="s">
         <v>320</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>321</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>322</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>323</v>
-      </c>
-      <c r="O3" t="s">
-        <v>324</v>
-      </c>
-      <c r="P3" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>628</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6924,31 +6924,31 @@
     </row>
     <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>678</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>679</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>485</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>486</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated integration test spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25CCC83-A216-AF44-88F4-A0057BF5D968}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3785C1D-8969-134F-A6E5-509E89F3D58B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1213,9 +1213,6 @@
     <t>cell_suspension.selected_cell_type.ontology_label</t>
   </si>
   <si>
-    <t>Total estimated cell count</t>
-  </si>
-  <si>
     <t>Protocol ID</t>
   </si>
   <si>
@@ -2141,6 +2138,9 @@
   </si>
   <si>
     <t>project.insdc_study_accessions</t>
+  </si>
+  <si>
+    <t>Estimated cell count</t>
   </si>
 </sst>
 </file>
@@ -2626,7 +2626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4:L4"/>
     </sheetView>
   </sheetViews>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2801,16 +2801,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>698</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>699</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2819,7 +2819,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2844,13 +2844,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>685</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>685</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>686</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2912,34 +2912,34 @@
   <sheetData>
     <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>471</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>534</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>111</v>
@@ -2948,7 +2948,7 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>111</v>
@@ -2993,13 +2993,13 @@
         <v>272</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>538</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>539</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>267</v>
@@ -3020,19 +3020,19 @@
         <v>272</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>111</v>
@@ -3041,7 +3041,7 @@
         <v>112</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>111</v>
@@ -3052,49 +3052,49 @@
     </row>
     <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>476</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>550</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>298</v>
@@ -3133,13 +3133,13 @@
         <v>303</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>553</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>298</v>
@@ -3160,51 +3160,51 @@
         <v>303</v>
       </c>
       <c r="AK2" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>479</v>
+      </c>
+      <c r="E3" t="s">
         <v>480</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>481</v>
       </c>
-      <c r="F3" t="s">
-        <v>482</v>
-      </c>
       <c r="G3" t="s">
+        <v>560</v>
+      </c>
+      <c r="I3" t="s">
         <v>561</v>
-      </c>
-      <c r="I3" t="s">
-        <v>562</v>
       </c>
       <c r="P3" t="s">
         <v>316</v>
@@ -3243,13 +3243,13 @@
         <v>321</v>
       </c>
       <c r="AB3" t="s">
+        <v>562</v>
+      </c>
+      <c r="AC3" t="s">
         <v>563</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>564</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>565</v>
       </c>
       <c r="AE3" t="s">
         <v>316</v>
@@ -3270,153 +3270,153 @@
         <v>321</v>
       </c>
       <c r="AK3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="AL3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AN3" t="s">
         <v>561</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>599</v>
-      </c>
       <c r="AO4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>559</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -3472,53 +3472,53 @@
     </row>
     <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>678</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>482</v>
-      </c>
       <c r="J6" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>600</v>
-      </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>603</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>604</v>
       </c>
       <c r="P6" s="7"/>
       <c r="AB6" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="AC6" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AD6" s="6" t="s">
         <v>606</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AL6" s="7" t="s">
         <v>607</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>608</v>
       </c>
       <c r="AM6" s="6">
         <v>0</v>
@@ -3527,13 +3527,13 @@
         <v>16</v>
       </c>
       <c r="AO6" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>609</v>
       </c>
-      <c r="AP6" s="6" t="s">
-        <v>610</v>
-      </c>
       <c r="AQ6" s="6" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
   </sheetData>
@@ -3559,25 +3559,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>471</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -3586,11 +3586,11 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>111</v>
@@ -3599,92 +3599,92 @@
         <v>112</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>476</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>479</v>
+      </c>
+      <c r="E3" t="s">
         <v>480</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>481</v>
       </c>
-      <c r="F3" t="s">
-        <v>482</v>
-      </c>
       <c r="J3" t="s">
+        <v>514</v>
+      </c>
+      <c r="O3" t="s">
         <v>515</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>516</v>
-      </c>
-      <c r="P3" t="s">
-        <v>517</v>
       </c>
       <c r="Q3" t="s">
         <v>195</v>
@@ -3695,58 +3695,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>525</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>526</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3774,49 +3774,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>681</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>482</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>529</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="M6" s="7" t="s">
-        <v>531</v>
-      </c>
       <c r="N6" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="O6" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>516</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>517</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -4310,13 +4310,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>650</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4530,13 +4530,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="AI4" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="AI4" s="3" t="s">
-        <v>650</v>
-      </c>
       <c r="AJ4" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>228</v>
@@ -4653,13 +4653,13 @@
     </row>
     <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>658</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>659</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>660</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4698,13 +4698,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>199</v>
@@ -4713,7 +4713,7 @@
         <v>241</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>242</v>
@@ -4737,19 +4737,19 @@
         <v>244</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AH6" t="s">
+        <v>692</v>
+      </c>
+      <c r="AI6" t="s">
         <v>693</v>
       </c>
-      <c r="AI6" t="s">
-        <v>694</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>203</v>
@@ -4987,13 +4987,13 @@
         <v>282</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>652</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>283</v>
@@ -5180,13 +5180,13 @@
         <v>282</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>651</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>652</v>
-      </c>
       <c r="T4" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>329</v>
@@ -5303,16 +5303,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>657</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>658</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>665</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>666</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5354,13 +5354,13 @@
         <v>350</v>
       </c>
       <c r="R6" t="s">
+        <v>692</v>
+      </c>
+      <c r="S6" t="s">
         <v>693</v>
       </c>
-      <c r="S6" t="s">
-        <v>694</v>
-      </c>
       <c r="T6" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>352</v>
@@ -5369,7 +5369,7 @@
         <v>353</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -5387,8 +5387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5580,13 +5580,13 @@
         <v>389</v>
       </c>
       <c r="AD2" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>391</v>
-      </c>
       <c r="AF2" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -5603,77 +5603,77 @@
         <v>192</v>
       </c>
       <c r="I3" t="s">
+        <v>391</v>
+      </c>
+      <c r="J3" t="s">
         <v>392</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>393</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>394</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>395</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>396</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>397</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>398</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>399</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>400</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>401</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>402</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AD3" t="s">
         <v>403</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>404</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>322</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>412</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>413</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>371</v>
@@ -5685,34 +5685,34 @@
         <v>373</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>422</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>423</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>384</v>
@@ -5733,13 +5733,13 @@
         <v>389</v>
       </c>
       <c r="AD4" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>425</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -5781,16 +5781,16 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>666</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>667</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>664</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>668</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>669</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5805,28 +5805,28 @@
         <v>192</v>
       </c>
       <c r="I6" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>393</v>
-      </c>
       <c r="K6" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="N6" s="6">
         <v>85.3</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q6" s="6">
         <v>10</v>
@@ -5835,16 +5835,16 @@
         <v>22</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="V6" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="W6" s="6" t="s">
         <v>402</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>403</v>
       </c>
       <c r="X6" s="6" t="s">
         <v>242</v>
@@ -5859,10 +5859,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -5899,28 +5899,28 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>436</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>437</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>368</v>
@@ -5929,96 +5929,96 @@
         <v>368</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
+        <v>446</v>
+      </c>
+      <c r="E3" t="s">
         <v>447</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>448</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>449</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>450</v>
-      </c>
-      <c r="H3" t="s">
-        <v>451</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" t="s">
         <v>460</v>
-      </c>
-      <c r="K4" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6038,19 +6038,19 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6059,33 +6059,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6094,33 +6094,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6129,16 +6129,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -6170,25 +6170,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>472</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6217,31 +6217,31 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>298</v>
@@ -6264,13 +6264,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>479</v>
+      </c>
+      <c r="E3" t="s">
         <v>480</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>481</v>
-      </c>
-      <c r="F3" t="s">
-        <v>482</v>
       </c>
       <c r="J3" t="s">
         <v>316</v>
@@ -6296,46 +6296,46 @@
         <v>347</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>492</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6360,31 +6360,31 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>672</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>482</v>
-      </c>
       <c r="G6" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>495</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>316</v>
@@ -6428,25 +6428,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>472</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6476,34 +6476,34 @@
     </row>
     <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>476</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>613</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>614</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>298</v>
@@ -6526,13 +6526,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>479</v>
+      </c>
+      <c r="E3" t="s">
         <v>480</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>481</v>
-      </c>
-      <c r="F3" t="s">
-        <v>482</v>
       </c>
       <c r="K3" t="s">
         <v>316</v>
@@ -6555,52 +6555,52 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>624</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>625</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6626,31 +6626,31 @@
     </row>
     <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>675</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>482</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>627</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>628</v>
-      </c>
       <c r="I6" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -6681,25 +6681,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>472</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6708,109 +6708,109 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>630</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>474</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>476</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>479</v>
+      </c>
+      <c r="E3" t="s">
         <v>480</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>481</v>
       </c>
-      <c r="F3" t="s">
-        <v>482</v>
-      </c>
       <c r="J3" t="s">
+        <v>637</v>
+      </c>
+      <c r="K3" t="s">
         <v>638</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>639</v>
-      </c>
-      <c r="L3" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>647</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6832,34 +6832,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>683</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>684</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>481</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>482</v>
-      </c>
       <c r="G6" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>627</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>628</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Update integration test spreadsheet.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3785C1D-8969-134F-A6E5-509E89F3D58B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C08F5B-5620-2B4C-838F-9BD15C31B065}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1312,9 +1312,6 @@
     <t>cell_suspension.growth_conditions.feeder_layer_type</t>
   </si>
   <si>
-    <t>cell_suspension.total_estimated_cells</t>
-  </si>
-  <si>
     <t>dissociation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -2141,6 +2138,9 @@
   </si>
   <si>
     <t>Estimated cell count</t>
+  </si>
+  <si>
+    <t>cell_suspension.estimated_cell_count</t>
   </si>
 </sst>
 </file>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2801,16 +2801,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>696</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>697</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>698</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2819,7 +2819,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2844,13 +2844,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>683</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>684</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>684</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>685</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2912,34 +2912,34 @@
   <sheetData>
     <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>533</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>534</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>111</v>
@@ -2948,7 +2948,7 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>111</v>
@@ -2993,13 +2993,13 @@
         <v>272</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>537</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>538</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>267</v>
@@ -3020,19 +3020,19 @@
         <v>272</v>
       </c>
       <c r="AK1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>539</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>540</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>111</v>
@@ -3041,7 +3041,7 @@
         <v>112</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>111</v>
@@ -3055,46 +3055,46 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>298</v>
@@ -3133,13 +3133,13 @@
         <v>303</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>551</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>552</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>298</v>
@@ -3160,51 +3160,51 @@
         <v>303</v>
       </c>
       <c r="AK2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" t="s">
         <v>479</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>480</v>
       </c>
-      <c r="F3" t="s">
-        <v>481</v>
-      </c>
       <c r="G3" t="s">
+        <v>559</v>
+      </c>
+      <c r="I3" t="s">
         <v>560</v>
-      </c>
-      <c r="I3" t="s">
-        <v>561</v>
       </c>
       <c r="P3" t="s">
         <v>316</v>
@@ -3243,13 +3243,13 @@
         <v>321</v>
       </c>
       <c r="AB3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AC3" t="s">
         <v>562</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>563</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>564</v>
       </c>
       <c r="AE3" t="s">
         <v>316</v>
@@ -3270,153 +3270,153 @@
         <v>321</v>
       </c>
       <c r="AK3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AL3" t="s">
+        <v>559</v>
+      </c>
+      <c r="AN3" t="s">
         <v>560</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="AN4" s="3" t="s">
-        <v>598</v>
-      </c>
       <c r="AO4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>558</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -3472,53 +3472,53 @@
     </row>
     <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>676</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>677</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>481</v>
-      </c>
       <c r="J6" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>599</v>
-      </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>602</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>603</v>
       </c>
       <c r="P6" s="7"/>
       <c r="AB6" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="AC6" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AD6" s="6" t="s">
         <v>605</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AL6" s="7" t="s">
         <v>606</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>607</v>
       </c>
       <c r="AM6" s="6">
         <v>0</v>
@@ -3527,13 +3527,13 @@
         <v>16</v>
       </c>
       <c r="AO6" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>608</v>
       </c>
-      <c r="AP6" s="6" t="s">
-        <v>609</v>
-      </c>
       <c r="AQ6" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -3559,25 +3559,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -3586,11 +3586,11 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>111</v>
@@ -3599,16 +3599,16 @@
         <v>112</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>500</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3616,75 +3616,75 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" t="s">
         <v>479</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>480</v>
       </c>
-      <c r="F3" t="s">
-        <v>481</v>
-      </c>
       <c r="J3" t="s">
+        <v>513</v>
+      </c>
+      <c r="O3" t="s">
         <v>514</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>515</v>
-      </c>
-      <c r="P3" t="s">
-        <v>516</v>
       </c>
       <c r="Q3" t="s">
         <v>195</v>
@@ -3695,58 +3695,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>524</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>525</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3774,49 +3774,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>679</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>680</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>481</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>527</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>528</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="M6" s="7" t="s">
         <v>529</v>
       </c>
-      <c r="M6" s="7" t="s">
-        <v>530</v>
-      </c>
       <c r="N6" s="7" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O6" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="P6" s="7" t="s">
         <v>515</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>516</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -4310,13 +4310,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>649</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4530,13 +4530,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="AI4" s="3" t="s">
         <v>648</v>
       </c>
-      <c r="AI4" s="3" t="s">
-        <v>649</v>
-      </c>
       <c r="AJ4" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>228</v>
@@ -4653,13 +4653,13 @@
     </row>
     <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>657</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>658</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>659</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4698,13 +4698,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>199</v>
@@ -4713,7 +4713,7 @@
         <v>241</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>242</v>
@@ -4737,19 +4737,19 @@
         <v>244</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AH6" t="s">
+        <v>691</v>
+      </c>
+      <c r="AI6" t="s">
         <v>692</v>
       </c>
-      <c r="AI6" t="s">
-        <v>693</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>203</v>
@@ -4987,13 +4987,13 @@
         <v>282</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>651</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>283</v>
@@ -5180,13 +5180,13 @@
         <v>282</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>651</v>
-      </c>
       <c r="T4" s="3" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>329</v>
@@ -5303,16 +5303,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>656</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>657</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>664</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>665</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5354,13 +5354,13 @@
         <v>350</v>
       </c>
       <c r="R6" t="s">
+        <v>691</v>
+      </c>
+      <c r="S6" t="s">
         <v>692</v>
       </c>
-      <c r="S6" t="s">
-        <v>693</v>
-      </c>
       <c r="T6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>352</v>
@@ -5369,7 +5369,7 @@
         <v>353</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -5388,7 +5388,7 @@
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5580,7 +5580,7 @@
         <v>389</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>390</v>
@@ -5733,13 +5733,13 @@
         <v>389</v>
       </c>
       <c r="AD4" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -5781,16 +5781,16 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>663</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>667</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>668</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5811,13 +5811,13 @@
         <v>392</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>427</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>428</v>
       </c>
       <c r="N6" s="6">
         <v>85.3</v>
@@ -5826,7 +5826,7 @@
         <v>394</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Q6" s="6">
         <v>10</v>
@@ -5838,7 +5838,7 @@
         <v>398</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="V6" s="6" t="s">
         <v>401</v>
@@ -5859,10 +5859,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -5899,28 +5899,28 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>368</v>
@@ -5929,33 +5929,33 @@
         <v>368</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>443</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>444</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>390</v>
@@ -5964,61 +5964,61 @@
         <v>390</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
+        <v>445</v>
+      </c>
+      <c r="E3" t="s">
         <v>446</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>447</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>448</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>449</v>
-      </c>
-      <c r="H3" t="s">
-        <v>450</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>404</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" t="s">
         <v>459</v>
-      </c>
-      <c r="K4" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6038,19 +6038,19 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6059,33 +6059,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6094,33 +6094,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6129,16 +6129,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -6170,25 +6170,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6220,28 +6220,28 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>478</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>298</v>
@@ -6264,13 +6264,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" t="s">
         <v>479</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>480</v>
-      </c>
-      <c r="F3" t="s">
-        <v>481</v>
       </c>
       <c r="J3" t="s">
         <v>316</v>
@@ -6296,46 +6296,46 @@
         <v>347</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6360,31 +6360,31 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>671</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>480</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>481</v>
-      </c>
       <c r="G6" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>493</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>494</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>316</v>
@@ -6428,25 +6428,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6479,31 +6479,31 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>612</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>613</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>298</v>
@@ -6526,13 +6526,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" t="s">
         <v>479</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>480</v>
-      </c>
-      <c r="F3" t="s">
-        <v>481</v>
       </c>
       <c r="K3" t="s">
         <v>316</v>
@@ -6555,52 +6555,52 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>624</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6626,31 +6626,31 @@
     </row>
     <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>674</v>
-      </c>
       <c r="D6" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>481</v>
-      </c>
       <c r="G6" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>627</v>
-      </c>
       <c r="I6" s="7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -6681,25 +6681,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6708,13 +6708,13 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6722,95 +6722,95 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>475</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>634</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>635</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" t="s">
         <v>479</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>480</v>
       </c>
-      <c r="F3" t="s">
-        <v>481</v>
-      </c>
       <c r="J3" t="s">
+        <v>636</v>
+      </c>
+      <c r="K3" t="s">
         <v>637</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>638</v>
-      </c>
-      <c r="L3" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>646</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6832,34 +6832,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>682</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>683</v>
-      </c>
       <c r="D6" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>479</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>481</v>
-      </c>
       <c r="G6" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>626</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>627</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Updated integration test spreadsheets.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3785C1D-8969-134F-A6E5-509E89F3D58B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450078E6-6974-CA4F-AE90-D98B77D23FEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -1351,9 +1351,6 @@
     <t>The length of a sequenced read in this file, in nucleotides.</t>
   </si>
   <si>
-    <t>An INSDC (International Nucleotide Sequence Database Collaboration) run accession. Can be from the DDBJ, NCBI, or EMBL-EBI. Accession must start with DRR, SRR, or ERR.</t>
-  </si>
-  <si>
     <t>A unique ID for the process.</t>
   </si>
   <si>
@@ -1375,9 +1372,6 @@
     <t>Read length</t>
   </si>
   <si>
-    <t>INSDC run</t>
-  </si>
-  <si>
     <t>Process ID</t>
   </si>
   <si>
@@ -1414,9 +1408,6 @@
     <t>sequence_file.read_length</t>
   </si>
   <si>
-    <t>sequence_file.insdc_run</t>
-  </si>
-  <si>
     <t>library_preparation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -2141,13 +2132,22 @@
   </si>
   <si>
     <t>Estimated cell count</t>
+  </si>
+  <si>
+    <t>sequence_file.insdc_run_accessions</t>
+  </si>
+  <si>
+    <t>INSDC run accession</t>
+  </si>
+  <si>
+    <t>An INSDC (International Nucleotide Sequence Database Collaboration) run accession from the DDBJ, NCBI, or EMBL-EBI.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2185,6 +2185,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2212,7 +2220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2241,6 +2249,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2686,7 +2697,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2801,16 +2812,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>695</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>697</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>698</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2819,7 +2830,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2844,13 +2855,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2912,34 +2923,34 @@
   <sheetData>
     <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>534</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>111</v>
@@ -2948,7 +2959,7 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>111</v>
@@ -2993,13 +3004,13 @@
         <v>272</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>267</v>
@@ -3020,19 +3031,19 @@
         <v>272</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AP1" s="1" t="s">
         <v>111</v>
@@ -3041,7 +3052,7 @@
         <v>112</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>111</v>
@@ -3055,46 +3066,46 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>546</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>549</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>298</v>
@@ -3133,13 +3144,13 @@
         <v>303</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>298</v>
@@ -3160,51 +3171,51 @@
         <v>303</v>
       </c>
       <c r="AK2" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="AP2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="AL2" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>556</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="I3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="P3" t="s">
         <v>316</v>
@@ -3243,13 +3254,13 @@
         <v>321</v>
       </c>
       <c r="AB3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="AC3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="AD3" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="AE3" t="s">
         <v>316</v>
@@ -3270,153 +3281,153 @@
         <v>321</v>
       </c>
       <c r="AK3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="AL3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="AN3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>546</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>547</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AL4" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>598</v>
-      </c>
       <c r="AO4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="AR4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>556</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
@@ -3472,53 +3483,53 @@
     </row>
     <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>596</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>600</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>599</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>601</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>602</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>603</v>
       </c>
       <c r="P6" s="7"/>
       <c r="AB6" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="AC6" s="6" t="s">
+        <v>602</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="AL6" s="7" t="s">
         <v>604</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>606</v>
-      </c>
-      <c r="AL6" s="7" t="s">
-        <v>607</v>
       </c>
       <c r="AM6" s="6">
         <v>0</v>
@@ -3527,13 +3538,13 @@
         <v>16</v>
       </c>
       <c r="AO6" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -3559,25 +3570,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -3586,11 +3597,11 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>111</v>
@@ -3599,16 +3610,16 @@
         <v>112</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3616,75 +3627,75 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J3" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="O3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P3" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q3" t="s">
         <v>195</v>
@@ -3695,58 +3706,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>519</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>521</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="O4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>523</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3774,49 +3785,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -4310,13 +4321,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>652</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4530,13 +4541,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="AI4" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
         <v>649</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>652</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>228</v>
@@ -4653,13 +4664,13 @@
     </row>
     <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4698,13 +4709,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>199</v>
@@ -4713,7 +4724,7 @@
         <v>241</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>242</v>
@@ -4737,19 +4748,19 @@
         <v>244</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="AH6" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="AI6" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="AJ6" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>203</v>
@@ -4987,13 +4998,13 @@
         <v>282</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>650</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>653</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>283</v>
@@ -5180,13 +5191,13 @@
         <v>282</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>650</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>653</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>329</v>
@@ -5303,16 +5314,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5354,13 +5365,13 @@
         <v>350</v>
       </c>
       <c r="R6" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="S6" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="T6" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>352</v>
@@ -5369,7 +5380,7 @@
         <v>353</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -5387,7 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
@@ -5580,7 +5591,7 @@
         <v>389</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>390</v>
@@ -5781,16 +5792,16 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5859,10 +5870,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>
@@ -5883,8 +5894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5919,8 +5930,8 @@
       <c r="G1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>436</v>
+      <c r="H1" s="13" t="s">
+        <v>699</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>368</v>
@@ -5929,33 +5940,33 @@
         <v>368</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>443</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>444</v>
+        <v>698</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>390</v>
@@ -5964,61 +5975,61 @@
         <v>390</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E3" t="s">
+        <v>445</v>
+      </c>
+      <c r="F3" t="s">
         <v>446</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>447</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>448</v>
-      </c>
-      <c r="G3" t="s">
-        <v>449</v>
-      </c>
-      <c r="H3" t="s">
-        <v>450</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>404</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="K4" t="s">
         <v>457</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="K4" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6038,19 +6049,19 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>687</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>690</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6059,33 +6070,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I6" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>678</v>
-      </c>
       <c r="K6" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>688</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>691</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6094,33 +6105,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I7" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>678</v>
-      </c>
       <c r="K7" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>686</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>666</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>689</v>
-      </c>
       <c r="E8" s="7" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6129,16 +6140,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I8" s="7" t="s">
+        <v>672</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>678</v>
-      </c>
       <c r="K8" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -6170,25 +6181,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6220,28 +6231,28 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>478</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>298</v>
@@ -6264,13 +6275,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J3" t="s">
         <v>316</v>
@@ -6296,46 +6307,46 @@
         <v>347</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6360,31 +6371,31 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>316</v>
@@ -6428,25 +6439,25 @@
   <sheetData>
     <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6479,31 +6490,31 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>610</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>613</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>298</v>
@@ -6526,13 +6537,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="K3" t="s">
         <v>316</v>
@@ -6558,49 +6569,49 @@
         <v>424</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>622</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6626,31 +6637,31 @@
     </row>
     <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -6681,25 +6692,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>468</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6708,13 +6719,13 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6722,57 +6733,57 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F3" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="J3" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="K3" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="L3" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6780,37 +6791,37 @@
         <v>425</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>644</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>645</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6832,34 +6843,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Update 10x test spreadsheet
Update spreadsheet to include the
correct values to match the updated
subscription query for 10xv2 data:
- Add library_construction_approach
  nucleic_acid_source: single cell
- Change library_construction_approach
  end_bias field to "3 prime tag"
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehsan/Devel/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C08F5B-5620-2B4C-838F-9BD15C31B065}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="Library preparation protocol" sheetId="9" r:id="rId10"/>
     <sheet name="Sequencing protocol" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="703">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -1852,9 +1851,6 @@
     <t>10X v2 sequencing</t>
   </si>
   <si>
-    <t>full length</t>
-  </si>
-  <si>
     <t>poly-dT</t>
   </si>
   <si>
@@ -2141,12 +2137,24 @@
   </si>
   <si>
     <t>cell_suspension.estimated_cell_count</t>
+  </si>
+  <si>
+    <t>3 prime tag</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol_json.nucleic_acid_source</t>
+  </si>
+  <si>
+    <t>single cell"</t>
+  </si>
+  <si>
+    <t>Source cells or organelles from which nucleic acid molecules were collected.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2623,7 +2631,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2686,7 +2694,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2801,16 +2809,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>695</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>696</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>697</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2819,7 +2827,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2842,15 +2850,15 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>682</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>682</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>683</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>683</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>684</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2892,25 +2900,24 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AU6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:AU5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="62" customWidth="1"/>
+    <col min="13" max="13" width="48" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>464</v>
       </c>
@@ -2948,109 +2955,112 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>390</v>
       </c>
@@ -3088,109 +3098,112 @@
         <v>545</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>478</v>
       </c>
@@ -3206,80 +3219,80 @@
       <c r="I3" t="s">
         <v>560</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>316</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>317</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>318</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>319</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>320</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>321</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>316</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>317</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>318</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>319</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>320</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>321</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>561</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>562</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>563</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>316</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>317</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>318</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>319</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>320</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>321</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>564</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>559</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>457</v>
       </c>
@@ -3317,109 +3330,112 @@
         <v>545</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="AT4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>53</v>
       </c>
@@ -3469,16 +3485,17 @@
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
       <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
     </row>
-    <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>674</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>675</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>676</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>478</v>
@@ -3498,57 +3515,55 @@
       <c r="L6" s="6" t="s">
         <v>598</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>600</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="AB6" s="6" t="s">
+      <c r="Q6" s="7"/>
+      <c r="AC6" s="6" t="s">
+        <v>699</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AE6" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AM6" s="7" t="s">
         <v>605</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AN6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="6">
+        <v>16</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>606</v>
-      </c>
-      <c r="AM6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="6">
-        <v>16</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>607</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>608</v>
       </c>
       <c r="AQ6" s="6" t="s">
         <v>607</v>
+      </c>
+      <c r="AR6" s="6" t="s">
+        <v>606</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3772,15 +3787,15 @@
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>677</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>678</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>679</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>478</v>
@@ -3828,16 +3843,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3850,7 +3860,7 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="135" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3993,7 +4003,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>97</v>
       </c>
@@ -4027,20 +4037,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
@@ -4310,13 +4315,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>648</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4530,13 +4535,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="AI4" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="AI4" s="3" t="s">
-        <v>648</v>
-      </c>
       <c r="AJ4" s="3" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>228</v>
@@ -4651,15 +4656,15 @@
       <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
     </row>
-    <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>656</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>657</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>658</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4698,13 +4703,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>199</v>
@@ -4713,7 +4718,7 @@
         <v>241</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>242</v>
@@ -4737,19 +4742,19 @@
         <v>244</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="AH6" t="s">
+        <v>690</v>
+      </c>
+      <c r="AI6" t="s">
         <v>691</v>
       </c>
-      <c r="AI6" t="s">
-        <v>692</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>203</v>
@@ -4788,16 +4793,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4987,13 +4987,13 @@
         <v>282</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>650</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>283</v>
@@ -5180,13 +5180,13 @@
         <v>282</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>650</v>
-      </c>
       <c r="T4" s="3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>329</v>
@@ -5301,18 +5301,18 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>655</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>662</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>656</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>663</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>664</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5354,13 +5354,13 @@
         <v>350</v>
       </c>
       <c r="R6" t="s">
+        <v>690</v>
+      </c>
+      <c r="S6" t="s">
         <v>691</v>
       </c>
-      <c r="S6" t="s">
-        <v>692</v>
-      </c>
       <c r="T6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>352</v>
@@ -5369,29 +5369,28 @@
         <v>353</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="29" max="29" width="28.1640625" customWidth="1"/>
+    <col min="30" max="30" width="30.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" s="1" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -5580,7 +5579,7 @@
         <v>389</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>390</v>
@@ -5733,7 +5732,7 @@
         <v>389</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>423</v>
@@ -5779,18 +5778,18 @@
       <c r="AF5" s="12"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>665</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>662</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>666</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>667</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5859,10 +5858,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
   </sheetData>
@@ -5871,16 +5870,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6036,18 +6030,18 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>445</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>460</v>
@@ -6062,27 +6056,27 @@
         <v>449</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>445</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>462</v>
@@ -6097,27 +6091,27 @@
         <v>449</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>445</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>463</v>
@@ -6132,10 +6126,10 @@
         <v>449</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>461</v>
@@ -6147,16 +6141,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6358,15 +6347,15 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>667</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>668</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>669</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>670</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>478</v>
@@ -6408,16 +6397,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6494,16 +6478,16 @@
         <v>474</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>611</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>612</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>298</v>
@@ -6558,49 +6542,49 @@
         <v>423</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>622</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>623</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6624,15 +6608,15 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>671</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>672</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>673</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>478</v>
@@ -6644,28 +6628,23 @@
         <v>480</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>626</v>
-      </c>
       <c r="I6" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6708,13 +6687,13 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>628</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6737,22 +6716,22 @@
         <v>474</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>634</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6766,13 +6745,13 @@
         <v>480</v>
       </c>
       <c r="J3" t="s">
+        <v>635</v>
+      </c>
+      <c r="K3" t="s">
         <v>636</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>637</v>
-      </c>
-      <c r="L3" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6780,37 +6759,37 @@
         <v>424</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>644</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>645</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6830,15 +6809,15 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>679</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>680</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>681</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>682</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>478</v>
@@ -6850,16 +6829,16 @@
         <v>480</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>624</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>625</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>626</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>
@@ -6871,10 +6850,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated 10x spreadsheet to match new pipelines query.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450078E6-6974-CA4F-AE90-D98B77D23FEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1490605-5D93-4841-8109-EFA6DD08FADC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="702">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -1846,9 +1846,6 @@
     <t>10X v2 sequencing</t>
   </si>
   <si>
-    <t>full length</t>
-  </si>
-  <si>
     <t>poly-dT</t>
   </si>
   <si>
@@ -2141,6 +2138,15 @@
   </si>
   <si>
     <t>An INSDC (International Nucleotide Sequence Database Collaboration) run accession from the DDBJ, NCBI, or EMBL-EBI.</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.nucleic_acid_source</t>
+  </si>
+  <si>
+    <t>single cell</t>
+  </si>
+  <si>
+    <t>3 prime tag</t>
   </si>
 </sst>
 </file>
@@ -2247,11 +2253,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2697,7 +2703,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2812,16 +2818,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>694</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>695</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2830,7 +2836,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2855,13 +2861,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>680</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>680</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>681</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>681</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>682</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2913,15 +2919,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AU6"/>
+  <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:AU5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:47" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>462</v>
       </c>
@@ -2967,101 +2973,102 @@
       <c r="O1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>536</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>390</v>
       </c>
@@ -3108,100 +3115,103 @@
         <v>546</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>476</v>
       </c>
@@ -3217,80 +3227,80 @@
       <c r="I3" t="s">
         <v>558</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>316</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>317</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>318</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>319</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>320</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>321</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>316</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>317</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>318</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>319</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>320</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>321</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>559</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>560</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>561</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>316</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>317</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>318</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>319</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>320</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>321</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>562</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>557</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>455</v>
       </c>
@@ -3337,100 +3347,103 @@
         <v>546</v>
       </c>
       <c r="P4" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>583</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>553</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AS4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="AS4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="AT4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>53</v>
       </c>
@@ -3480,16 +3493,17 @@
       <c r="AS5" s="8"/>
       <c r="AT5" s="8"/>
       <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
     </row>
-    <row r="6" spans="1:47" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>671</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>672</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>673</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>674</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>476</v>
@@ -3518,33 +3532,36 @@
       <c r="O6" s="6" t="s">
         <v>600</v>
       </c>
-      <c r="P6" s="7"/>
-      <c r="AB6" s="6" t="s">
+      <c r="P6" s="6" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="AC6" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="AD6" s="6" t="s">
         <v>601</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AE6" s="6" t="s">
         <v>602</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AM6" s="7" t="s">
         <v>603</v>
       </c>
-      <c r="AL6" s="7" t="s">
+      <c r="AN6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="6">
+        <v>16</v>
+      </c>
+      <c r="AP6" s="6" t="s">
         <v>604</v>
-      </c>
-      <c r="AM6" s="6">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="6">
-        <v>16</v>
-      </c>
-      <c r="AO6" s="6" t="s">
-        <v>605</v>
-      </c>
-      <c r="AP6" s="6" t="s">
-        <v>606</v>
       </c>
       <c r="AQ6" s="6" t="s">
         <v>605</v>
+      </c>
+      <c r="AR6" s="6" t="s">
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -3785,13 +3802,13 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>674</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>676</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>677</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>476</v>
@@ -4321,13 +4338,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>646</v>
-      </c>
       <c r="AJ2" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4541,13 +4558,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="AI4" s="3" t="s">
         <v>645</v>
       </c>
-      <c r="AI4" s="3" t="s">
-        <v>646</v>
-      </c>
       <c r="AJ4" s="3" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>228</v>
@@ -4664,13 +4681,13 @@
     </row>
     <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>654</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>655</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>656</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4709,13 +4726,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>199</v>
@@ -4724,7 +4741,7 @@
         <v>241</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>242</v>
@@ -4748,19 +4765,19 @@
         <v>244</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AH6" t="s">
+        <v>688</v>
+      </c>
+      <c r="AI6" t="s">
         <v>689</v>
       </c>
-      <c r="AI6" t="s">
-        <v>690</v>
-      </c>
       <c r="AJ6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>203</v>
@@ -4998,13 +5015,13 @@
         <v>282</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="S2" s="2" t="s">
-        <v>648</v>
-      </c>
       <c r="T2" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>283</v>
@@ -5191,13 +5208,13 @@
         <v>282</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>647</v>
       </c>
-      <c r="S4" s="3" t="s">
-        <v>648</v>
-      </c>
       <c r="T4" s="3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>329</v>
@@ -5314,16 +5331,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>660</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>654</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>661</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>662</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5365,13 +5382,13 @@
         <v>350</v>
       </c>
       <c r="R6" t="s">
+        <v>688</v>
+      </c>
+      <c r="S6" t="s">
         <v>689</v>
       </c>
-      <c r="S6" t="s">
-        <v>690</v>
-      </c>
       <c r="T6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>352</v>
@@ -5380,7 +5397,7 @@
         <v>353</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
   </sheetData>
@@ -5591,7 +5608,7 @@
         <v>389</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>390</v>
@@ -5786,22 +5803,22 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
       <c r="AG5" s="3"/>
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>659</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>663</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>660</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>664</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>665</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5870,10 +5887,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>
@@ -5894,7 +5911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -5930,8 +5947,8 @@
       <c r="G1" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>699</v>
+      <c r="H1" s="12" t="s">
+        <v>698</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>368</v>
@@ -5966,7 +5983,7 @@
         <v>442</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>390</v>
@@ -6020,7 +6037,7 @@
         <v>454</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>455</v>
@@ -6044,21 +6061,21 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>444</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>458</v>
@@ -6073,10 +6090,10 @@
         <v>448</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>459</v>
@@ -6084,16 +6101,16 @@
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>444</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>460</v>
@@ -6108,10 +6125,10 @@
         <v>448</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>459</v>
@@ -6119,16 +6136,16 @@
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>444</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>461</v>
@@ -6143,10 +6160,10 @@
         <v>448</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>459</v>
@@ -6371,13 +6388,13 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>665</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>666</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>667</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>668</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>476</v>
@@ -6505,16 +6522,16 @@
         <v>472</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>609</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>610</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>298</v>
@@ -6569,49 +6586,49 @@
         <v>424</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>607</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>621</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -6637,13 +6654,13 @@
     </row>
     <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>668</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>670</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>671</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>476</v>
@@ -6655,13 +6672,13 @@
         <v>478</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>623</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>624</v>
-      </c>
       <c r="I6" s="7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -6719,13 +6736,13 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6748,22 +6765,22 @@
         <v>472</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>630</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>631</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>632</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6777,13 +6794,13 @@
         <v>478</v>
       </c>
       <c r="J3" t="s">
+        <v>633</v>
+      </c>
+      <c r="K3" t="s">
         <v>634</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>635</v>
-      </c>
-      <c r="L3" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6791,37 +6808,37 @@
         <v>425</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>637</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>638</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>639</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>640</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>628</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>630</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>642</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>643</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6843,13 +6860,13 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>679</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>680</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>476</v>
@@ -6861,16 +6878,16 @@
         <v>478</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>623</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>624</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Hotfixes to integration test spreadsheets.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1490605-5D93-4841-8109-EFA6DD08FADC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9642EF-9BDF-0743-BC54-46A20B376798}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="30940" windowHeight="18800" tabRatio="993" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="706">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -1312,9 +1312,6 @@
     <t>cell_suspension.growth_conditions.feeder_layer_type</t>
   </si>
   <si>
-    <t>cell_suspension.total_estimated_cells</t>
-  </si>
-  <si>
     <t>dissociation_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
@@ -1495,24 +1492,6 @@
     <t>collection_protocol.protocol_core.document</t>
   </si>
   <si>
-    <t>collection_protocol.protocol_reagents.retail_name</t>
-  </si>
-  <si>
-    <t>collection_protocol.protocol_reagents.catalog_number</t>
-  </si>
-  <si>
-    <t>collection_protocol.protocol_reagents.manufacturer</t>
-  </si>
-  <si>
-    <t>collection_protocol.protocol_reagents.lot_number</t>
-  </si>
-  <si>
-    <t>collection_protocol.protocol_reagents.expiry_date</t>
-  </si>
-  <si>
-    <t>collection_protocol.protocol_reagents.kit_titer</t>
-  </si>
-  <si>
     <t>organ extraction</t>
   </si>
   <si>
@@ -1870,9 +1849,6 @@
     <t>dissociation_protocol.dissociation_method.ontology_label</t>
   </si>
   <si>
-    <t>dissociation_protocol.nucleic_acid_source.user_friendly</t>
-  </si>
-  <si>
     <t>dissociation_protocol.protocol_core.protocol_name</t>
   </si>
   <si>
@@ -1888,27 +1864,6 @@
     <t>dissociation_protocol.protocol_core.document</t>
   </si>
   <si>
-    <t>dissociation_protocol.nucleic_acid_source</t>
-  </si>
-  <si>
-    <t>dissociation_protocol.protocol_reagents.retail_name</t>
-  </si>
-  <si>
-    <t>dissociation_protocol.protocol_reagents.catalog_number</t>
-  </si>
-  <si>
-    <t>dissociation_protocol.protocol_reagents.manufacturer</t>
-  </si>
-  <si>
-    <t>dissociation_protocol.protocol_reagents.lot_number</t>
-  </si>
-  <si>
-    <t>dissociation_protocol.protocol_reagents.expiry_date</t>
-  </si>
-  <si>
-    <t>dissociation_protocol.protocol_reagents.kit_titer</t>
-  </si>
-  <si>
     <t>fluorescence-activated cell sorting</t>
   </si>
   <si>
@@ -2147,6 +2102,63 @@
   </si>
   <si>
     <t>3 prime tag</t>
+  </si>
+  <si>
+    <t>cell_suspension.estimated_cell_count</t>
+  </si>
+  <si>
+    <t>collection_protocol.method.text</t>
+  </si>
+  <si>
+    <t>collection_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>collection_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>collection_protocol.reagents.retail_name</t>
+  </si>
+  <si>
+    <t>collection_protocol.reagents.catalog_number</t>
+  </si>
+  <si>
+    <t>collection_protocol.reagents.manufacturer</t>
+  </si>
+  <si>
+    <t>collection_protocol.reagents.lot_number</t>
+  </si>
+  <si>
+    <t>collection_protocol.reagents.expiry_date</t>
+  </si>
+  <si>
+    <t>collection_protocol.reagents.kit_titer</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.method.text</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>dissociation_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.library_construction_method.text</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.library_construction_method.ontology</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.library_construction_method.ontology_label</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.method.text</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>sequencing_protocol.method.ontology_label</t>
   </si>
 </sst>
 </file>
@@ -2703,7 +2715,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>650</v>
+        <v>635</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2818,16 +2830,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>691</v>
+        <v>676</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>692</v>
+        <v>677</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>693</v>
+        <v>678</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>694</v>
+        <v>679</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2836,7 +2848,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>690</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2861,13 +2873,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>680</v>
+        <v>665</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>680</v>
+        <v>665</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>681</v>
+        <v>666</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2921,42 +2933,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>111</v>
@@ -2965,7 +2977,7 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>111</v>
@@ -3011,13 +3023,13 @@
         <v>272</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>267</v>
@@ -3038,19 +3050,19 @@
         <v>272</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>111</v>
@@ -3059,7 +3071,7 @@
         <v>112</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>111</v>
@@ -3073,49 +3085,49 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>546</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>699</v>
+        <v>684</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>298</v>
@@ -3154,13 +3166,13 @@
         <v>303</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>298</v>
@@ -3181,51 +3193,51 @@
         <v>303</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="AT2" s="2" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E3" t="s">
         <v>476</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>477</v>
       </c>
-      <c r="F3" t="s">
-        <v>478</v>
-      </c>
       <c r="G3" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="I3" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="Q3" t="s">
         <v>316</v>
@@ -3264,13 +3276,13 @@
         <v>321</v>
       </c>
       <c r="AC3" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="AD3" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="AE3" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="AF3" t="s">
         <v>316</v>
@@ -3291,156 +3303,156 @@
         <v>321</v>
       </c>
       <c r="AL3" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="AM3" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="AO3" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>699</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>574</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>589</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>591</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>593</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>594</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>553</v>
-      </c>
       <c r="AS4" s="3" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
@@ -3497,56 +3509,56 @@
     </row>
     <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>673</v>
+        <v>658</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>478</v>
-      </c>
       <c r="J6" s="6" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="AC6" s="6" t="s">
-        <v>701</v>
+        <v>686</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="AN6" s="6">
         <v>0</v>
@@ -3555,13 +3567,13 @@
         <v>16</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="AR6" s="6" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -3580,32 +3592,32 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>467</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -3614,11 +3626,11 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>111</v>
@@ -3627,16 +3639,16 @@
         <v>112</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3644,75 +3656,75 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E3" t="s">
         <v>476</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>477</v>
       </c>
-      <c r="F3" t="s">
-        <v>478</v>
-      </c>
       <c r="J3" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="O3" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="P3" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="Q3" t="s">
         <v>195</v>
@@ -3723,58 +3735,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>703</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>516</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>517</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>503</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>520</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3802,49 +3814,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>675</v>
+        <v>660</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>676</v>
+        <v>661</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>478</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -4338,13 +4350,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4558,13 +4570,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>644</v>
+        <v>629</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>648</v>
+        <v>633</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>228</v>
@@ -4681,13 +4693,13 @@
     </row>
     <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>654</v>
+        <v>639</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>655</v>
+        <v>640</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4726,13 +4738,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>656</v>
+        <v>641</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>657</v>
+        <v>642</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>199</v>
@@ -4741,7 +4753,7 @@
         <v>241</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>658</v>
+        <v>643</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>242</v>
@@ -4765,19 +4777,19 @@
         <v>244</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>652</v>
+        <v>637</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>651</v>
+        <v>636</v>
       </c>
       <c r="AH6" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="AI6" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="AJ6" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="AN6" s="7" t="s">
         <v>203</v>
@@ -5015,13 +5027,13 @@
         <v>282</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>283</v>
@@ -5208,13 +5220,13 @@
         <v>282</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>646</v>
+        <v>631</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>647</v>
+        <v>632</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>649</v>
+        <v>634</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>329</v>
@@ -5331,16 +5343,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>659</v>
+        <v>644</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>653</v>
+        <v>638</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>660</v>
+        <v>645</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>661</v>
+        <v>646</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5382,13 +5394,13 @@
         <v>350</v>
       </c>
       <c r="R6" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="S6" t="s">
-        <v>689</v>
+        <v>674</v>
       </c>
       <c r="T6" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>352</v>
@@ -5397,7 +5409,7 @@
         <v>353</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>
@@ -5415,8 +5427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5608,7 +5620,7 @@
         <v>389</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>695</v>
+        <v>680</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>390</v>
@@ -5761,13 +5773,13 @@
         <v>389</v>
       </c>
       <c r="AD4" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -5809,16 +5821,16 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>659</v>
+        <v>644</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>663</v>
+        <v>648</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>664</v>
+        <v>649</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5839,13 +5851,13 @@
         <v>392</v>
       </c>
       <c r="K6" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>427</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>428</v>
       </c>
       <c r="N6" s="6">
         <v>85.3</v>
@@ -5854,7 +5866,7 @@
         <v>394</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Q6" s="6">
         <v>10</v>
@@ -5866,7 +5878,7 @@
         <v>398</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="V6" s="6" t="s">
         <v>401</v>
@@ -5887,10 +5899,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>677</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>
@@ -5927,28 +5939,28 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>435</v>
-      </c>
       <c r="H1" s="12" t="s">
-        <v>698</v>
+        <v>683</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>368</v>
@@ -5957,33 +5969,33 @@
         <v>368</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>442</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>697</v>
+        <v>682</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>390</v>
@@ -5992,61 +6004,61 @@
         <v>390</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
+        <v>443</v>
+      </c>
+      <c r="E3" t="s">
         <v>444</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>445</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>446</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>447</v>
-      </c>
-      <c r="H3" t="s">
-        <v>448</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>404</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>696</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" t="s">
         <v>456</v>
-      </c>
-      <c r="K4" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6066,19 +6078,19 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>683</v>
+        <v>668</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>686</v>
+        <v>671</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6087,33 +6099,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>684</v>
+        <v>669</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>687</v>
+        <v>672</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6122,33 +6134,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>682</v>
+        <v>667</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>662</v>
+        <v>647</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6157,16 +6169,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>674</v>
+        <v>659</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -6188,7 +6200,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6198,25 +6210,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>468</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6248,28 +6260,28 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>475</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>298</v>
@@ -6292,13 +6304,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E3" t="s">
         <v>476</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>477</v>
-      </c>
-      <c r="F3" t="s">
-        <v>478</v>
       </c>
       <c r="J3" t="s">
         <v>316</v>
@@ -6324,46 +6336,46 @@
         <v>347</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>483</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>473</v>
+        <v>688</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>474</v>
+        <v>689</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>475</v>
+        <v>690</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>484</v>
+        <v>691</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>485</v>
+        <v>692</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>486</v>
+        <v>693</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>487</v>
+        <v>694</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>488</v>
+        <v>695</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>489</v>
+        <v>696</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6388,31 +6400,31 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>665</v>
+        <v>650</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>667</v>
+        <v>652</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>478</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>316</v>
@@ -6446,35 +6458,35 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>468</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6482,156 +6494,77 @@
       <c r="I1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>272</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E3" t="s">
+        <v>476</v>
+      </c>
+      <c r="F3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>303</v>
+      <c r="G4" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>699</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>476</v>
-      </c>
-      <c r="E3" t="s">
-        <v>477</v>
-      </c>
-      <c r="F3" t="s">
-        <v>478</v>
-      </c>
-      <c r="K3" t="s">
-        <v>316</v>
-      </c>
-      <c r="L3" t="s">
-        <v>317</v>
-      </c>
-      <c r="M3" t="s">
-        <v>318</v>
-      </c>
-      <c r="N3" t="s">
-        <v>319</v>
-      </c>
-      <c r="O3" t="s">
-        <v>320</v>
-      </c>
-      <c r="P3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>614</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>607</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>620</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>53</v>
       </c>
@@ -6643,42 +6576,34 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>668</v>
+        <v>653</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>669</v>
+        <v>654</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>478</v>
-      </c>
       <c r="G6" s="7" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>623</v>
+        <v>608</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -6709,25 +6634,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>467</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>468</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6736,13 +6661,13 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>624</v>
+        <v>609</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>625</v>
+        <v>610</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>626</v>
+        <v>611</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6750,95 +6675,95 @@
         <v>390</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>470</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>627</v>
+        <v>612</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>628</v>
+        <v>613</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>629</v>
+        <v>614</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>630</v>
+        <v>615</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>631</v>
+        <v>616</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>475</v>
+      </c>
+      <c r="E3" t="s">
         <v>476</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>477</v>
       </c>
-      <c r="F3" t="s">
-        <v>478</v>
-      </c>
       <c r="J3" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="K3" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
       <c r="L3" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>637</v>
+        <v>622</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>638</v>
+        <v>623</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>639</v>
+        <v>624</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>640</v>
+        <v>625</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>627</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>628</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>629</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6860,34 +6785,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>677</v>
+        <v>662</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>678</v>
+        <v>663</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>679</v>
+        <v>664</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>476</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>477</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>478</v>
-      </c>
       <c r="G6" s="6" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>623</v>
+        <v>608</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Fix typo in nucleic_acid_source field
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="28660" windowHeight="16580" tabRatio="993" activeTab="9"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28880" windowHeight="19240" tabRatio="993" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -2142,13 +2142,13 @@
     <t>3 prime tag</t>
   </si>
   <si>
-    <t>library_preparation_protocol_json.nucleic_acid_source</t>
-  </si>
-  <si>
-    <t>single cell"</t>
-  </si>
-  <si>
     <t>Source cells or organelles from which nucleic acid molecules were collected.</t>
+  </si>
+  <si>
+    <t>single cell</t>
+  </si>
+  <si>
+    <t>library_preparation_protocol.nucleic_acid_source</t>
   </si>
 </sst>
 </file>
@@ -2908,7 +2908,7 @@
   <dimension ref="A1:AV6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2955,7 +2955,7 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>534</v>
@@ -3098,7 +3098,7 @@
         <v>545</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>546</v>
@@ -3330,7 +3330,7 @@
         <v>545</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>546</v>

</xml_diff>

<commit_message>
Hot fix edited tab names to test new generic tab implementation
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehsan/Devel/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F404FB-D9A5-9F4A-939B-A82B347C07F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="28880" windowHeight="19240" tabRatio="993" activeTab="9"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28880" windowHeight="19240" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
-    <sheet name="Contact" sheetId="2" r:id="rId2"/>
+    <sheet name="Project - Contact" sheetId="2" r:id="rId2"/>
     <sheet name="Donor organism" sheetId="3" r:id="rId3"/>
     <sheet name="Specimen from organism" sheetId="4" r:id="rId4"/>
     <sheet name="Cell suspension" sheetId="5" r:id="rId5"/>
@@ -24,7 +25,7 @@
     <sheet name="Library preparation protocol" sheetId="9" r:id="rId10"/>
     <sheet name="Sequencing protocol" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2154,7 +2155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2631,7 +2632,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2850,7 +2851,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>682</v>
       </c>
@@ -2904,10 +2905,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -3487,7 +3488,7 @@
       <c r="AU5" s="8"/>
       <c r="AV5" s="8"/>
     </row>
-    <row r="6" spans="1:48" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>673</v>
       </c>
@@ -3563,7 +3564,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3787,7 +3788,7 @@
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>676</v>
       </c>
@@ -3847,10 +3848,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3860,7 +3861,7 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="135" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -4003,7 +4004,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>97</v>
       </c>
@@ -4037,7 +4038,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4045,7 +4046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
@@ -4656,7 +4657,7 @@
       <c r="BA5" s="8"/>
       <c r="BB5" s="8"/>
     </row>
-    <row r="6" spans="1:55" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>655</v>
       </c>
@@ -4797,7 +4798,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5301,7 +5302,7 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>661</v>
       </c>
@@ -5379,7 +5380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
@@ -5778,7 +5779,7 @@
       <c r="AF5" s="12"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>664</v>
       </c>
@@ -5874,7 +5875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6030,7 +6031,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>685</v>
       </c>
@@ -6065,7 +6066,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>686</v>
       </c>
@@ -6100,7 +6101,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>684</v>
       </c>
@@ -6145,7 +6146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6347,7 +6348,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>667</v>
       </c>
@@ -6401,7 +6402,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6608,7 +6609,7 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
     </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>670</v>
       </c>
@@ -6644,7 +6645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6809,7 +6810,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>679</v>
       </c>

</xml_diff>

<commit_message>
rolling back hot fix due to extra errors
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F404FB-D9A5-9F4A-939B-A82B347C07F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0949BE8-5DA5-F941-B77C-4B99269A9B46}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="28880" windowHeight="19240" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28880" windowHeight="19240" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
-    <sheet name="Project - Contact" sheetId="2" r:id="rId2"/>
+    <sheet name="Contact" sheetId="2" r:id="rId2"/>
     <sheet name="Donor organism" sheetId="3" r:id="rId3"/>
     <sheet name="Specimen from organism" sheetId="4" r:id="rId4"/>
     <sheet name="Cell suspension" sheetId="5" r:id="rId5"/>
@@ -3851,7 +3851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -4049,8 +4049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6:AJ6"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD28" sqref="AD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updataed terms to latest
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9642EF-9BDF-0743-BC54-46A20B376798}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E7A794-C1C5-6448-B6BD-3F7234991AA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="30940" windowHeight="18800" tabRatio="993" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="460" windowWidth="30940" windowHeight="18800" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
-    <sheet name="Contact" sheetId="2" r:id="rId2"/>
+    <sheet name="Project - Contributors" sheetId="2" r:id="rId2"/>
     <sheet name="Donor organism" sheetId="3" r:id="rId3"/>
     <sheet name="Specimen from organism" sheetId="4" r:id="rId4"/>
     <sheet name="Cell suspension" sheetId="5" r:id="rId5"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="706">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="698">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -556,15 +556,6 @@
     <t>donor_organism.development_stage.ontology_label</t>
   </si>
   <si>
-    <t>donor_organism.familial_relationship.is_child_of.user_friendly</t>
-  </si>
-  <si>
-    <t>donor_organism.familial_relationship.is_parent_of.user_friendly</t>
-  </si>
-  <si>
-    <t>donor_organism.familial_relationship.is_sibling_of.user_friendly</t>
-  </si>
-  <si>
     <t>Gestational age</t>
   </si>
   <si>
@@ -592,9 +583,6 @@
     <t>Is living?</t>
   </si>
   <si>
-    <t>donor_organism.biological_sex.user_friendly</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -727,15 +715,6 @@
     <t>donor_organism.organism_age</t>
   </si>
   <si>
-    <t>donor_organism.familial_relationship.is_child_of</t>
-  </si>
-  <si>
-    <t>donor_organism.familial_relationship.is_parent_of</t>
-  </si>
-  <si>
-    <t>donor_organism.familial_relationship.is_sibling_of</t>
-  </si>
-  <si>
     <t>donor_organism.gestational_age</t>
   </si>
   <si>
@@ -745,9 +724,6 @@
     <t>donor_organism.is_living</t>
   </si>
   <si>
-    <t>donor_organism.biological_sex</t>
-  </si>
-  <si>
     <t>donor_organism.weight</t>
   </si>
   <si>
@@ -1036,9 +1012,6 @@
     <t>specimen_from_organism.state_of_specimen.gross_description</t>
   </si>
   <si>
-    <t>specimen_from_organism.state_of_specimen.gross_image</t>
-  </si>
-  <si>
     <t>specimen_from_organism.state_of_specimen.ischemic_temperature</t>
   </si>
   <si>
@@ -1048,9 +1021,6 @@
     <t>specimen_from_organism.state_of_specimen.microscopic_description</t>
   </si>
   <si>
-    <t>specimen_from_organism.state_of_specimen.microscopic_image</t>
-  </si>
-  <si>
     <t>specimen_from_organism.state_of_specimen.postmortem_interval</t>
   </si>
   <si>
@@ -2159,6 +2129,12 @@
   </si>
   <si>
     <t>sequencing_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.gross_images</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.state_of_specimen.microscopic_images</t>
   </si>
 </sst>
 </file>
@@ -2715,7 +2691,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2830,16 +2806,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2848,7 +2824,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2873,13 +2849,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2941,34 +2917,34 @@
   <sheetData>
     <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>111</v>
@@ -2977,7 +2953,7 @@
         <v>112</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>111</v>
@@ -2987,82 +2963,82 @@
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>111</v>
@@ -3071,7 +3047,7 @@
         <v>112</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>111</v>
@@ -3082,377 +3058,377 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AD2" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AP2" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E3" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F3" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="G3" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="I3" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="Q3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="R3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="S3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="T3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="U3" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="V3" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="W3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="X3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="Y3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="Z3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="AA3" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="AB3" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="AC3" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="AD3" t="s">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="AE3" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="AF3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="AG3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="AH3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="AI3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="AJ3" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="AK3" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="AL3" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="AM3" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="AO3" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="AR4" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>700</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>701</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>702</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>564</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>565</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>573</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>574</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>578</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>580</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>582</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>585</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>588</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>544</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>545</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>546</v>
-      </c>
       <c r="AS4" s="3" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
@@ -3509,56 +3485,56 @@
     </row>
     <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="AC6" s="6" t="s">
-        <v>686</v>
+        <v>676</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="AN6" s="6">
         <v>0</v>
@@ -3567,13 +3543,13 @@
         <v>16</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="AR6" s="6" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -3599,25 +3575,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -3626,11 +3602,11 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>111</v>
@@ -3639,95 +3615,95 @@
         <v>112</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>493</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E3" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F3" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="J3" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="O3" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="P3" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="Q3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="R3" t="s">
         <v>84</v>
@@ -3735,58 +3711,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>703</v>
+        <v>693</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>704</v>
+        <v>694</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3814,49 +3790,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -4081,10 +4057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BC6"/>
+  <dimension ref="A1:AY6"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6:AJ6"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AT1" sqref="AT1:AT1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4092,7 +4068,7 @@
     <col min="31" max="31" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:51" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
@@ -4201,55 +4177,51 @@
       <c r="AJ1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
+      <c r="AK1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="AN1" s="1" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="AP1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AR1" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="AS1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AT1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AV1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AW1" s="1"/>
       <c r="AX1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BB1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="BC1" s="1"/>
+      <c r="AY1" s="1"/>
     </row>
-    <row r="2" spans="1:55" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:51" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>138</v>
       </c>
@@ -4350,13 +4322,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4400,99 +4372,87 @@
       <c r="AX2" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="AY2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
         <v>185</v>
       </c>
-      <c r="AZ2" s="2" t="s">
+      <c r="E3" t="s">
         <v>186</v>
       </c>
-      <c r="BA2" s="2" t="s">
+      <c r="F3" t="s">
         <v>187</v>
       </c>
-      <c r="BB2" s="2" t="s">
+      <c r="G3" t="s">
         <v>188</v>
       </c>
+      <c r="H3" t="s">
+        <v>189</v>
+      </c>
+      <c r="M3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N3" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>193</v>
+      </c>
+      <c r="R3" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T3" t="s">
+        <v>196</v>
+      </c>
+      <c r="U3" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>202</v>
+      </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F3" t="s">
-        <v>191</v>
-      </c>
-      <c r="G3" t="s">
-        <v>192</v>
-      </c>
-      <c r="H3" t="s">
-        <v>193</v>
-      </c>
-      <c r="M3" t="s">
-        <v>194</v>
-      </c>
-      <c r="N3" t="s">
-        <v>195</v>
-      </c>
-      <c r="P3" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>197</v>
-      </c>
-      <c r="R3" t="s">
-        <v>198</v>
-      </c>
-      <c r="S3" t="s">
-        <v>199</v>
-      </c>
-      <c r="T3" t="s">
-        <v>200</v>
-      </c>
-      <c r="U3" t="s">
-        <v>201</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>202</v>
-      </c>
-      <c r="AN3" t="s">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="B4" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="C4" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="D4" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>210</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>214</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>146</v>
@@ -4504,40 +4464,40 @@
         <v>148</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>226</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>161</v>
@@ -4549,7 +4509,7 @@
         <v>163</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>165</v>
@@ -4570,28 +4530,28 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AL4" s="3" t="s">
-        <v>229</v>
+        <v>172</v>
       </c>
       <c r="AM4" s="3" t="s">
-        <v>230</v>
+        <v>173</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="AP4" s="3" t="s">
         <v>176</v>
@@ -4600,40 +4560,28 @@
         <v>177</v>
       </c>
       <c r="AR4" s="3" t="s">
-        <v>232</v>
+        <v>178</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>179</v>
+        <v>226</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>180</v>
+        <v>227</v>
       </c>
       <c r="AU4" s="3" t="s">
         <v>181</v>
       </c>
       <c r="AV4" s="3" t="s">
-        <v>233</v>
+        <v>182</v>
       </c>
       <c r="AW4" s="3" t="s">
-        <v>234</v>
+        <v>183</v>
       </c>
       <c r="AX4" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="AY4" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="AZ4" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="BA4" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BB4" s="3" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>53</v>
       </c>
@@ -4686,47 +4634,43 @@
       <c r="AV5" s="8"/>
       <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
-      <c r="AY5" s="8"/>
-      <c r="AZ5" s="8"/>
-      <c r="BA5" s="8"/>
-      <c r="BB5" s="8"/>
     </row>
-    <row r="6" spans="1:55" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="H6" s="7">
         <v>36.4</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>101</v>
@@ -4738,91 +4682,91 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="Z6" s="7" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="AA6" s="7">
         <v>20</v>
       </c>
       <c r="AB6" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC6" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AD6" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="AE6" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>663</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>664</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>663</v>
+      </c>
+      <c r="AK6" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO6" s="7">
+        <v>160</v>
+      </c>
+      <c r="AP6" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AR6" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="AS6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT6" s="7">
+        <v>60</v>
+      </c>
+      <c r="AU6" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="AV6" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="AW6" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="AX6" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="AC6" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="AE6" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="AF6" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>673</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>674</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>673</v>
-      </c>
-      <c r="AN6" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="AR6" s="7">
-        <v>160</v>
-      </c>
-      <c r="AS6" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="AT6" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="AU6" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="AV6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="AX6" s="7">
-        <v>60</v>
-      </c>
-      <c r="AY6" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="AZ6" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="BA6" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="BB6" s="7" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -4840,8 +4784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6:T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4884,7 +4828,7 @@
         <v>129</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>112</v>
@@ -4893,7 +4837,7 @@
         <v>129</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>112</v>
@@ -4908,34 +4852,34 @@
         <v>112</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>127</v>
@@ -4947,31 +4891,31 @@
         <v>112</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5000,299 +4944,299 @@
         <v>144</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="U3" t="s">
+        <v>297</v>
+      </c>
+      <c r="W3" t="s">
+        <v>298</v>
+      </c>
+      <c r="X3" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>300</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>301</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>302</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>303</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>304</v>
+      </c>
+      <c r="AD3" t="s">
         <v>305</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AH3" t="s">
         <v>306</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AI3" t="s">
         <v>307</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AJ3" t="s">
         <v>308</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AK3" t="s">
         <v>309</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AL3" t="s">
         <v>310</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AM3" t="s">
         <v>311</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AN3" t="s">
         <v>312</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AO3" t="s">
         <v>313</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>314</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>315</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>316</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>317</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>318</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>319</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>320</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="V4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="W4" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>632</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="AH4" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>337</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>342</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.2">
@@ -5343,73 +5287,73 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="R6" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="S6" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="T6" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -5459,10 +5403,10 @@
         <v>108</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>133</v>
@@ -5474,34 +5418,34 @@
         <v>112</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>125</v>
@@ -5513,7 +5457,7 @@
         <v>112</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>111</v>
@@ -5522,13 +5466,13 @@
         <v>112</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5557,229 +5501,229 @@
         <v>144</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>680</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>390</v>
-      </c>
       <c r="AF2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I3" t="s">
+        <v>381</v>
+      </c>
+      <c r="J3" t="s">
+        <v>382</v>
+      </c>
+      <c r="N3" t="s">
+        <v>383</v>
+      </c>
+      <c r="O3" t="s">
+        <v>384</v>
+      </c>
+      <c r="P3" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>386</v>
+      </c>
+      <c r="R3" t="s">
+        <v>387</v>
+      </c>
+      <c r="S3" t="s">
+        <v>388</v>
+      </c>
+      <c r="T3" t="s">
+        <v>389</v>
+      </c>
+      <c r="U3" t="s">
+        <v>390</v>
+      </c>
+      <c r="V3" t="s">
         <v>391</v>
       </c>
-      <c r="J3" t="s">
+      <c r="W3" t="s">
         <v>392</v>
       </c>
-      <c r="N3" t="s">
+      <c r="AD3" t="s">
         <v>393</v>
-      </c>
-      <c r="O3" t="s">
-        <v>394</v>
-      </c>
-      <c r="P3" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>396</v>
-      </c>
-      <c r="R3" t="s">
-        <v>397</v>
-      </c>
-      <c r="S3" t="s">
-        <v>398</v>
-      </c>
-      <c r="T3" t="s">
-        <v>399</v>
-      </c>
-      <c r="U3" t="s">
-        <v>400</v>
-      </c>
-      <c r="V3" t="s">
-        <v>401</v>
-      </c>
-      <c r="W3" t="s">
-        <v>402</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>403</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>413</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>414</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -5821,52 +5765,52 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="N6" s="6">
         <v>85.3</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="Q6" s="6">
         <v>10</v>
@@ -5875,34 +5819,34 @@
         <v>22</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="AD6" s="11">
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -5939,126 +5883,126 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>438</v>
+        <v>428</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>439</v>
+        <v>429</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>440</v>
+        <v>430</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>442</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="E3" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
       <c r="F3" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="G3" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
       <c r="H3" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
       <c r="K4" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6078,19 +6022,19 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6099,33 +6043,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6134,33 +6078,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6169,16 +6113,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -6210,25 +6154,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6237,145 +6181,145 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>472</v>
+        <v>462</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E3" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F3" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="J3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="K3" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="L3" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="M3" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="N3" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="O3" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>693</v>
+        <v>683</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>694</v>
+        <v>684</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>695</v>
+        <v>685</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>696</v>
+        <v>686</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6400,49 +6344,49 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -6460,7 +6404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -6468,25 +6412,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6497,71 +6441,71 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E3" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F3" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>697</v>
+        <v>687</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -6579,31 +6523,31 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -6634,25 +6578,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -6661,109 +6605,109 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>469</v>
+        <v>459</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>470</v>
+        <v>460</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E3" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F3" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="J3" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
       <c r="K3" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="L3" t="s">
-        <v>620</v>
+        <v>610</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>621</v>
+        <v>611</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>628</v>
+        <v>618</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6785,34 +6729,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>597</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>608</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>607</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>618</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Update integration test spreadsheets
Change library_construction_approach
to library_construction_method in test
spreadsheets to be consistent with the
schema
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehsan/Devel/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E7A794-C1C5-6448-B6BD-3F7234991AA2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="460" windowWidth="30940" windowHeight="18800" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42520" yWindow="460" windowWidth="30940" windowHeight="18800" tabRatio="993" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="Library preparation protocol" sheetId="9" r:id="rId10"/>
     <sheet name="Sequencing protocol" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="695">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -1622,15 +1621,6 @@
   </si>
   <si>
     <t>library_preparation_protocol.input_nucleic_acid_molecule.ontology_label</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.library_construction_approach.text</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.library_construction_approach.ontology</t>
-  </si>
-  <si>
-    <t>library_preparation_protocol.library_construction_approach.ontology_label</t>
   </si>
   <si>
     <t>End bias</t>
@@ -2140,7 +2130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2628,7 +2618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2691,7 +2681,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2806,16 +2796,16 @@
         <v>50</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>666</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>669</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>51</v>
@@ -2824,7 +2814,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2847,15 +2837,15 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>54</v>
@@ -2897,23 +2887,25 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="12" max="12" width="27.83203125" customWidth="1"/>
+    <col min="13" max="13" width="52.1640625" customWidth="1"/>
+    <col min="14" max="14" width="56.33203125" customWidth="1"/>
+    <col min="15" max="15" width="69.83203125" customWidth="1"/>
+    <col min="16" max="16" width="45.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -3094,16 +3086,16 @@
         <v>526</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>527</v>
+        <v>687</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>528</v>
+        <v>688</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>529</v>
+        <v>689</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>290</v>
@@ -3142,13 +3134,13 @@
         <v>295</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>290</v>
@@ -3169,7 +3161,7 @@
         <v>295</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="AM2" s="2" t="s">
         <v>521</v>
@@ -3181,22 +3173,22 @@
         <v>523</v>
       </c>
       <c r="AP2" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AS2" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>536</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
@@ -3210,10 +3202,10 @@
         <v>467</v>
       </c>
       <c r="G3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I3" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="Q3" t="s">
         <v>308</v>
@@ -3252,13 +3244,13 @@
         <v>313</v>
       </c>
       <c r="AC3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="AD3" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="AE3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AF3" t="s">
         <v>308</v>
@@ -3279,13 +3271,13 @@
         <v>313</v>
       </c>
       <c r="AL3" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="AM3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AO3" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
@@ -3293,28 +3285,28 @@
         <v>444</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>553</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>524</v>
@@ -3326,109 +3318,109 @@
         <v>526</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="Q4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>557</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>559</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AB4" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>564</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AH4" s="3" t="s">
         <v>568</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="AG4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>572</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>574</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="AM4" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>578</v>
-      </c>
       <c r="AP4" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="AS4" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="AQ4" s="3" t="s">
+      <c r="AT4" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="AR4" s="3" t="s">
+      <c r="AU4" s="3" t="s">
         <v>536</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
@@ -3483,15 +3475,15 @@
       <c r="AU5" s="8"/>
       <c r="AV5" s="8"/>
     </row>
-    <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>465</v>
@@ -3503,38 +3495,38 @@
         <v>467</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="N6" s="7" t="s">
         <v>579</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="O6" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>579</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>581</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>582</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>583</v>
-      </c>
       <c r="P6" s="6" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="AC6" s="6" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="AN6" s="6">
         <v>0</v>
@@ -3543,28 +3535,23 @@
         <v>16</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="AR6" s="6" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3744,13 +3731,13 @@
         <v>486</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>503</v>
@@ -3788,15 +3775,15 @@
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>465</v>
@@ -3844,16 +3831,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3866,7 +3848,7 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="135" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -4009,7 +3991,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>97</v>
       </c>
@@ -4043,20 +4025,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY6"/>
   <sheetViews>
     <sheetView topLeftCell="AG1" workbookViewId="0">
@@ -4322,13 +4299,13 @@
         <v>170</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AI2" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
         <v>620</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>623</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>171</v>
@@ -4530,13 +4507,13 @@
         <v>170</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="AI4" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>623</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>224</v>
@@ -4635,15 +4612,15 @@
       <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
     </row>
-    <row r="6" spans="1:51" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4682,13 +4659,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>232</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>195</v>
@@ -4697,7 +4674,7 @@
         <v>233</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>234</v>
@@ -4721,19 +4698,19 @@
         <v>236</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="AH6" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="AI6" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="AJ6" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="AK6" s="7" t="s">
         <v>199</v>
@@ -4772,19 +4749,14 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
@@ -4971,13 +4943,13 @@
         <v>274</v>
       </c>
       <c r="R2" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>624</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>275</v>
@@ -5164,13 +5136,13 @@
         <v>274</v>
       </c>
       <c r="R4" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>621</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>622</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>624</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>321</v>
@@ -5179,7 +5151,7 @@
         <v>322</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>323</v>
@@ -5191,7 +5163,7 @@
         <v>325</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>326</v>
@@ -5285,18 +5257,18 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5338,13 +5310,13 @@
         <v>340</v>
       </c>
       <c r="R6" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="S6" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="T6" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>342</v>
@@ -5353,22 +5325,17 @@
         <v>343</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -5564,7 +5531,7 @@
         <v>379</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>380</v>
@@ -5717,7 +5684,7 @@
         <v>379</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>413</v>
@@ -5763,18 +5730,18 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5843,10 +5810,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -5855,16 +5822,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5904,7 +5866,7 @@
         <v>424</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>358</v>
@@ -5939,7 +5901,7 @@
         <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>380</v>
@@ -5993,7 +5955,7 @@
         <v>443</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>444</v>
@@ -6020,18 +5982,18 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>433</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>447</v>
@@ -6046,27 +6008,27 @@
         <v>437</v>
       </c>
       <c r="I6" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>646</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>433</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>449</v>
@@ -6081,27 +6043,27 @@
         <v>437</v>
       </c>
       <c r="I7" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>646</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>433</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>450</v>
@@ -6116,10 +6078,10 @@
         <v>437</v>
       </c>
       <c r="I8" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>646</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>649</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>448</v>
@@ -6131,16 +6093,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6295,31 +6252,31 @@
         <v>472</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>683</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6342,15 +6299,15 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>465</v>
@@ -6392,16 +6349,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6459,13 +6411,13 @@
         <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -6484,28 +6436,28 @@
         <v>413</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>594</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>596</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -6521,15 +6473,15 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>465</v>
@@ -6541,28 +6493,23 @@
         <v>467</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6605,13 +6552,13 @@
         <v>112</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6634,22 +6581,22 @@
         <v>461</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -6663,13 +6610,13 @@
         <v>467</v>
       </c>
       <c r="J3" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="K3" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="L3" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -6677,37 +6624,37 @@
         <v>414</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>611</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>614</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>615</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>603</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>604</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6727,15 +6674,15 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>465</v>
@@ -6747,16 +6694,16 @@
         <v>467</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>
@@ -6768,10 +6715,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated integration test sheets to organ_parts.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sehsan/Devel/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B6EE2B-C09B-BA42-B8CF-378BE5208079}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42520" yWindow="460" windowWidth="30940" windowHeight="18800" tabRatio="993" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27380" tabRatio="993" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <sheet name="Library preparation protocol" sheetId="9" r:id="rId10"/>
     <sheet name="Sequencing protocol" sheetId="8" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="698">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -2125,12 +2126,21 @@
   </si>
   <si>
     <t>specimen_from_organism.state_of_specimen.microscopic_images</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ_parts.text</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ_parts.ontology</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.organ_parts.ontology_label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2618,7 +2628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2837,7 +2847,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="6" customFormat="1" ht="150" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>652</v>
       </c>
@@ -2891,10 +2901,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AV6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -3475,7 +3485,7 @@
       <c r="AU5" s="8"/>
       <c r="AV5" s="8"/>
     </row>
-    <row r="6" spans="1:48" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>643</v>
       </c>
@@ -3551,7 +3561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3775,7 +3785,7 @@
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
     </row>
-    <row r="6" spans="1:19" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>646</v>
       </c>
@@ -3835,7 +3845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3848,7 +3858,7 @@
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="135" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -3991,7 +4001,7 @@
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>97</v>
       </c>
@@ -4025,7 +4035,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4033,7 +4043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY6"/>
   <sheetViews>
     <sheetView topLeftCell="AG1" workbookViewId="0">
@@ -4612,7 +4622,7 @@
       <c r="AW5" s="8"/>
       <c r="AX5" s="8"/>
     </row>
-    <row r="6" spans="1:51" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>625</v>
       </c>
@@ -4753,11 +4763,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AP6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5127,13 +5137,13 @@
         <v>271</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>272</v>
+        <v>695</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>273</v>
+        <v>696</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>274</v>
+        <v>697</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>618</v>
@@ -5257,7 +5267,7 @@
       <c r="AO5" s="8"/>
       <c r="AP5" s="8"/>
     </row>
-    <row r="6" spans="1:42" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>631</v>
       </c>
@@ -5335,7 +5345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
@@ -5730,7 +5740,7 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>634</v>
       </c>
@@ -5826,7 +5836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5982,7 +5992,7 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>655</v>
       </c>
@@ -6017,7 +6027,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>656</v>
       </c>
@@ -6052,7 +6062,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>654</v>
       </c>
@@ -6097,7 +6107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6299,7 +6309,7 @@
       <c r="O5" s="8"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="1:16" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>637</v>
       </c>
@@ -6353,7 +6363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6473,7 +6483,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>640</v>
       </c>
@@ -6509,7 +6519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6674,7 +6684,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>649</v>
       </c>

</xml_diff>

<commit_message>
added new nested tab names
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hewgreen/google_drive_EBI/hca_clones/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B5F129-208C-2649-A5A8-96FCA2A90824}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FE3D10-3309-BC49-810E-07ABB261FCE8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
-    <sheet name="Contact" sheetId="2" r:id="rId2"/>
+    <sheet name="Project - Contact" sheetId="2" r:id="rId2"/>
     <sheet name="Donor organism" sheetId="3" r:id="rId3"/>
     <sheet name="Specimen from organism" sheetId="4" r:id="rId4"/>
     <sheet name="Cell suspension" sheetId="5" r:id="rId5"/>

</xml_diff>

<commit_message>
Updated integration test spraedsheets.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ABB034-951A-084F-AD27-445025469EE7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38F207-9BB1-9845-8688-8999FD26664F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14860" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14860" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -658,12 +658,6 @@
     <t>donor_organism.biomaterial_core.genotype</t>
   </si>
   <si>
-    <t>donor_organism.biomaterial_core.biosd_biomaterial</t>
-  </si>
-  <si>
-    <t>donor_organism.biomaterial_core.insdc_biomaterial</t>
-  </si>
-  <si>
     <t>donor_organism.human_specific.body_mass_index</t>
   </si>
   <si>
@@ -991,12 +985,6 @@
     <t>specimen_from_organism.biomaterial_core.genotype</t>
   </si>
   <si>
-    <t>specimen_from_organism.biomaterial_core.biosd_biomaterial</t>
-  </si>
-  <si>
-    <t>specimen_from_organism.biomaterial_core.insdc_biomaterial</t>
-  </si>
-  <si>
     <t>specimen_from_organism.state_of_specimen.autolysis_score</t>
   </si>
   <si>
@@ -1231,12 +1219,6 @@
     <t>cell_suspension.biomaterial_core.genotype</t>
   </si>
   <si>
-    <t>cell_suspension.biomaterial_core.biosd_biomaterial</t>
-  </si>
-  <si>
-    <t>cell_suspension.biomaterial_core.insdc_biomaterial</t>
-  </si>
-  <si>
     <t>cell_suspension.cell_morphology.cell_morphology</t>
   </si>
   <si>
@@ -2135,6 +2117,24 @@
   </si>
   <si>
     <t>project.publications.title</t>
+  </si>
+  <si>
+    <t>donor_organism.biomaterial_core.biosamples_accession</t>
+  </si>
+  <si>
+    <t>donor_organism.biomaterial_core.insdc_sample_accession</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.biomaterial_core.biosamples_accession</t>
+  </si>
+  <si>
+    <t>specimen_from_organism.biomaterial_core.insdc_sample_accession</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.biosamples_accession</t>
+  </si>
+  <si>
+    <t>cell_suspension.biomaterial_core.insdc_sample_accession</t>
   </si>
 </sst>
 </file>
@@ -2638,7 +2638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2801,7 +2801,7 @@
         <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>697</v>
+        <v>691</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>47</v>
@@ -2810,19 +2810,19 @@
         <v>48</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>696</v>
+        <v>690</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>49</v>
@@ -2831,7 +2831,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2856,13 +2856,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>52</v>
@@ -2926,34 +2926,34 @@
   <sheetData>
     <row r="1" spans="1:48" ht="85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>108</v>
@@ -2962,7 +2962,7 @@
         <v>109</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>108</v>
@@ -2972,82 +2972,82 @@
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="AC1" s="1" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>261</v>
-      </c>
       <c r="AL1" s="1" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="AQ1" s="1" t="s">
         <v>108</v>
@@ -3056,7 +3056,7 @@
         <v>109</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="AT1" s="1" t="s">
         <v>108</v>
@@ -3067,377 +3067,377 @@
     </row>
     <row r="2" spans="1:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="AP2" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>686</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="AF2" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>527</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G3" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="I3" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="Q3" t="s">
+        <v>303</v>
+      </c>
+      <c r="R3" t="s">
+        <v>304</v>
+      </c>
+      <c r="S3" t="s">
         <v>305</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>306</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>307</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>308</v>
       </c>
-      <c r="U3" t="s">
-        <v>309</v>
-      </c>
-      <c r="V3" t="s">
-        <v>310</v>
-      </c>
       <c r="W3" t="s">
+        <v>303</v>
+      </c>
+      <c r="X3" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y3" t="s">
         <v>305</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>306</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>307</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>308</v>
       </c>
-      <c r="AA3" t="s">
-        <v>309</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>310</v>
-      </c>
       <c r="AC3" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AD3" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="AE3" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="AF3" t="s">
+        <v>303</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>304</v>
+      </c>
+      <c r="AH3" t="s">
         <v>305</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AI3" t="s">
         <v>306</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AJ3" t="s">
         <v>307</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AK3" t="s">
         <v>308</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>309</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>310</v>
-      </c>
       <c r="AL3" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="AM3" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="AO3" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>542</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="K4" s="3" t="s">
+      <c r="W4" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="AP4" s="3" t="s">
         <v>522</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="AQ4" s="3" t="s">
         <v>523</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>685</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>686</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>548</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>549</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>550</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>551</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>553</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>554</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>558</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>559</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>560</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>561</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>562</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>564</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>565</v>
-      </c>
-      <c r="AI4" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="AJ4" s="3" t="s">
-        <v>567</v>
-      </c>
-      <c r="AK4" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="AL4" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>570</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>529</v>
-      </c>
       <c r="AR4" s="3" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="AU4" s="3" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
@@ -3494,56 +3494,56 @@
     </row>
     <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="AC6" s="6" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="AN6" s="6">
         <v>0</v>
@@ -3552,13 +3552,13 @@
         <v>16</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="AR6" s="6" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
   </sheetData>
@@ -3579,25 +3579,25 @@
   <sheetData>
     <row r="1" spans="1:19" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>108</v>
@@ -3606,11 +3606,11 @@
         <v>109</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>108</v>
@@ -3619,92 +3619,92 @@
         <v>109</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="J3" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="O3" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="P3" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="Q3" t="s">
         <v>188</v>
@@ -3715,58 +3715,58 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>495</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>497</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>688</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>689</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -3794,49 +3794,49 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>98</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="Q6" s="7">
         <v>4</v>
@@ -3987,7 +3987,7 @@
         <v>92</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>93</v>
@@ -4053,8 +4053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY6"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AN17" sqref="AN17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4316,13 +4316,13 @@
         <v>167</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>168</v>
@@ -4439,14 +4439,14 @@
       <c r="E4" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
+        <v>692</v>
+      </c>
+      <c r="G4" t="s">
+        <v>693</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>143</v>
@@ -4458,40 +4458,40 @@
         <v>145</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>158</v>
@@ -4503,7 +4503,7 @@
         <v>160</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>162</v>
@@ -4524,16 +4524,16 @@
         <v>167</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AL4" s="3" t="s">
         <v>169</v>
@@ -4545,7 +4545,7 @@
         <v>171</v>
       </c>
       <c r="AO4" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AP4" s="3" t="s">
         <v>173</v>
@@ -4557,10 +4557,10 @@
         <v>175</v>
       </c>
       <c r="AS4" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="AT4" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AU4" s="3" t="s">
         <v>178</v>
@@ -4572,7 +4572,7 @@
         <v>180</v>
       </c>
       <c r="AX4" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.2">
@@ -4631,13 +4631,13 @@
     </row>
     <row r="6" spans="1:51" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4655,16 +4655,16 @@
         <v>36.4</v>
       </c>
       <c r="I6" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="M6" s="7" t="s">
         <v>98</v>
@@ -4676,58 +4676,58 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>192</v>
       </c>
       <c r="T6" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="U6" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="X6" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y6" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="U6" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="X6" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="Y6" s="7" t="s">
-        <v>232</v>
-      </c>
       <c r="Z6" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AA6" s="7">
         <v>20</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="AH6" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="AI6" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="AJ6" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="AK6" s="7" t="s">
         <v>196</v>
@@ -4736,13 +4736,13 @@
         <v>160</v>
       </c>
       <c r="AP6" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="AQ6" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="AR6" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="AQ6" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="AR6" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="AS6" s="7" t="s">
         <v>98</v>
@@ -4751,16 +4751,16 @@
         <v>60</v>
       </c>
       <c r="AU6" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="AV6" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="AW6" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="AV6" s="7" t="s">
+      <c r="AX6" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="AW6" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="AX6" s="7" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4774,7 +4774,7 @@
   <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4817,7 +4817,7 @@
         <v>126</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>109</v>
@@ -4826,7 +4826,7 @@
         <v>126</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>109</v>
@@ -4841,34 +4841,34 @@
         <v>109</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>253</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>124</v>
@@ -4880,31 +4880,31 @@
         <v>109</v>
       </c>
       <c r="AH1" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:42" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4933,106 +4933,106 @@
         <v>141</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.2">
@@ -5049,183 +5049,183 @@
         <v>185</v>
       </c>
       <c r="U3" t="s">
+        <v>292</v>
+      </c>
+      <c r="W3" t="s">
+        <v>293</v>
+      </c>
+      <c r="X3" t="s">
         <v>294</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>295</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>296</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>297</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>298</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
         <v>299</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AD3" t="s">
         <v>300</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AH3" t="s">
         <v>301</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AI3" t="s">
         <v>302</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AJ3" t="s">
         <v>303</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AK3" t="s">
         <v>304</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AL3" t="s">
         <v>305</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AM3" t="s">
         <v>306</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AN3" t="s">
         <v>307</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AO3" t="s">
         <v>308</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>309</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>200</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>694</v>
+      </c>
+      <c r="H4" t="s">
+        <v>695</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="W4" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="X4" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>692</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>694</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>615</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>616</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>618</v>
-      </c>
-      <c r="U4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="AA4" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="AB4" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="W4" s="3" t="s">
-        <v>690</v>
-      </c>
-      <c r="X4" s="3" t="s">
+      <c r="AC4" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AD4" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH4" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="AA4" s="3" t="s">
-        <v>691</v>
-      </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AI4" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AJ4" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AK4" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="AE4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="AH4" s="3" t="s">
+      <c r="AL4" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="AI4" s="3" t="s">
+      <c r="AM4" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="AJ4" s="3" t="s">
+      <c r="AN4" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AO4" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AP4" s="3" t="s">
         <v>330</v>
-      </c>
-      <c r="AM4" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.2">
@@ -5276,16 +5276,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5300,49 +5300,49 @@
         <v>185</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="L6" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="O6" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q6" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="R6" t="s">
+        <v>651</v>
+      </c>
+      <c r="S6" t="s">
+        <v>652</v>
+      </c>
+      <c r="T6" t="s">
+        <v>651</v>
+      </c>
+      <c r="U6" s="7" t="s">
         <v>335</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="V6" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="N6" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="R6" t="s">
-        <v>657</v>
-      </c>
-      <c r="S6" t="s">
-        <v>658</v>
-      </c>
-      <c r="T6" t="s">
-        <v>657</v>
-      </c>
-      <c r="U6" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="V6" s="7" t="s">
-        <v>340</v>
-      </c>
       <c r="AP6" s="7" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -5355,8 +5355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AD5" sqref="AD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5387,10 +5387,10 @@
         <v>105</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>130</v>
@@ -5402,34 +5402,34 @@
         <v>109</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>122</v>
@@ -5441,7 +5441,7 @@
         <v>109</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>108</v>
@@ -5450,13 +5450,13 @@
         <v>109</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:33" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -5485,76 +5485,76 @@
         <v>141</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="AE2" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>664</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="AF2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -5571,143 +5571,143 @@
         <v>185</v>
       </c>
       <c r="I3" t="s">
+        <v>374</v>
+      </c>
+      <c r="J3" t="s">
+        <v>375</v>
+      </c>
+      <c r="N3" t="s">
+        <v>376</v>
+      </c>
+      <c r="O3" t="s">
+        <v>377</v>
+      </c>
+      <c r="P3" t="s">
         <v>378</v>
       </c>
-      <c r="J3" t="s">
+      <c r="Q3" t="s">
         <v>379</v>
       </c>
-      <c r="N3" t="s">
+      <c r="R3" t="s">
         <v>380</v>
       </c>
-      <c r="O3" t="s">
+      <c r="S3" t="s">
         <v>381</v>
       </c>
-      <c r="P3" t="s">
+      <c r="T3" t="s">
         <v>382</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
         <v>383</v>
       </c>
-      <c r="R3" t="s">
+      <c r="V3" t="s">
         <v>384</v>
       </c>
-      <c r="S3" t="s">
+      <c r="W3" t="s">
         <v>385</v>
       </c>
-      <c r="T3" t="s">
+      <c r="AD3" t="s">
         <v>386</v>
-      </c>
-      <c r="U3" t="s">
-        <v>387</v>
-      </c>
-      <c r="V3" t="s">
-        <v>388</v>
-      </c>
-      <c r="W3" t="s">
-        <v>389</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>390</v>
       </c>
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>696</v>
+      </c>
+      <c r="H4" t="s">
+        <v>697</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>393</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>359</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="N4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="X4" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>405</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
@@ -5749,16 +5749,16 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5773,28 +5773,28 @@
         <v>185</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="N6" s="6">
         <v>85.3</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="Q6" s="6">
         <v>10</v>
@@ -5803,34 +5803,34 @@
         <v>22</v>
       </c>
       <c r="S6" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>409</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="W6" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="U6" s="6" t="s">
-        <v>415</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="W6" s="6" t="s">
-        <v>389</v>
-      </c>
       <c r="X6" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AD6" s="11">
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -5862,126 +5862,126 @@
   <sheetData>
     <row r="1" spans="1:11" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="E3" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="F3" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="G3" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="H3" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="K4" t="s">
         <v>437</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="K4" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6001,19 +6001,19 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -6022,33 +6022,33 @@
         <v>26</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -6057,33 +6057,33 @@
         <v>98</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="K7" s="7" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="F8" s="7">
         <v>1</v>
@@ -6092,16 +6092,16 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -6128,25 +6128,25 @@
   <sheetData>
     <row r="1" spans="1:16" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>108</v>
@@ -6155,145 +6155,145 @@
         <v>109</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="J3" t="s">
+        <v>303</v>
+      </c>
+      <c r="K3" t="s">
+        <v>304</v>
+      </c>
+      <c r="L3" t="s">
         <v>305</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>306</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>307</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>308</v>
-      </c>
-      <c r="N3" t="s">
-        <v>309</v>
-      </c>
-      <c r="O3" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>674</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>675</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6318,49 +6318,49 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>470</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="J6" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="M6" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>308</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>310</v>
       </c>
     </row>
   </sheetData>
@@ -6381,25 +6381,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>108</v>
@@ -6410,71 +6410,71 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -6492,31 +6492,31 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -6542,25 +6542,25 @@
   <sheetData>
     <row r="1" spans="1:13" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>454</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>108</v>
@@ -6569,109 +6569,109 @@
         <v>109</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F3" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="J3" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="K3" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="L3" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>605</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>606</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>607</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>609</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>596</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>597</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>598</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>610</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6693,34 +6693,34 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="K6" s="6">
         <v>70</v>

</xml_diff>

<commit_message>
Updated integration testing spreadsheets.
</commit_message>
<xml_diff>
--- a/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
+++ b/infrastructure_testing_files/current/dcp_integration_test_metadata_1_10X_bundle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfreeberg/git/metadata-schema/infrastructure_testing_files/current/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D38F207-9BB1-9845-8688-8999FD26664F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F709F7-6941-144B-8CF7-614FF504741C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14860" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14860" yWindow="460" windowWidth="28800" windowHeight="16580" tabRatio="993" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="701">
   <si>
     <t>A short name for the project.</t>
   </si>
@@ -1858,12 +1858,6 @@
     <t>enrichment_protocol.markers</t>
   </si>
   <si>
-    <t>enrichment_protocol.min_size_selected</t>
-  </si>
-  <si>
-    <t>enrichment_protocol.max_size_selected</t>
-  </si>
-  <si>
     <t>donor_organism.diseases.text</t>
   </si>
   <si>
@@ -2135,6 +2129,21 @@
   </si>
   <si>
     <t>cell_suspension.biomaterial_core.insdc_sample_accession</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.method.text</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.method.ontology</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.method.ontology_label</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.minimum_size</t>
+  </si>
+  <si>
+    <t>enrichment_protocol.maximum_size</t>
   </si>
 </sst>
 </file>
@@ -2698,7 +2707,7 @@
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -2801,7 +2810,7 @@
         <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>47</v>
@@ -2810,19 +2819,19 @@
         <v>48</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>654</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>655</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>657</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>49</v>
@@ -2831,7 +2840,7 @@
         <v>50</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2856,13 +2865,13 @@
     </row>
     <row r="6" spans="1:16" s="6" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>52</v>
@@ -3103,16 +3112,16 @@
         <v>517</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>680</v>
-      </c>
       <c r="P2" s="2" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>285</v>
@@ -3335,16 +3344,16 @@
         <v>517</v>
       </c>
       <c r="M4" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="N4" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>680</v>
-      </c>
       <c r="P4" s="3" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>542</v>
@@ -3494,13 +3503,13 @@
     </row>
     <row r="6" spans="1:48" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>634</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>635</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>636</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>456</v>
@@ -3530,11 +3539,11 @@
         <v>571</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="Q6" s="7"/>
       <c r="AC6" s="6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="AD6" s="6" t="s">
         <v>572</v>
@@ -3748,13 +3757,13 @@
         <v>477</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>681</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>683</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>494</v>
@@ -3794,13 +3803,13 @@
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>637</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>638</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>639</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>456</v>
@@ -3987,7 +3996,7 @@
         <v>92</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>93</v>
@@ -4316,13 +4325,13 @@
         <v>167</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AK2" s="2" t="s">
         <v>168</v>
@@ -4440,10 +4449,10 @@
         <v>204</v>
       </c>
       <c r="F4" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G4" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>205</v>
@@ -4524,13 +4533,13 @@
         <v>167</v>
       </c>
       <c r="AH4" s="3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AK4" s="3" t="s">
         <v>219</v>
@@ -4631,13 +4640,13 @@
     </row>
     <row r="6" spans="1:51" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>616</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>617</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>618</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
@@ -4676,13 +4685,13 @@
         <v>0</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="Q6" s="7" t="s">
         <v>227</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>192</v>
@@ -4691,7 +4700,7 @@
         <v>228</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="X6" s="7" t="s">
         <v>229</v>
@@ -4715,19 +4724,19 @@
         <v>231</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="AH6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="AI6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="AJ6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="AK6" s="7" t="s">
         <v>196</v>
@@ -4960,13 +4969,13 @@
         <v>269</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>610</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>612</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>270</v>
@@ -5120,10 +5129,10 @@
         <v>313</v>
       </c>
       <c r="G4" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H4" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>261</v>
@@ -5144,22 +5153,22 @@
         <v>266</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>686</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>688</v>
-      </c>
       <c r="R4" s="3" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="S4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="T4" s="3" t="s">
         <v>610</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>612</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>314</v>
@@ -5168,7 +5177,7 @@
         <v>315</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>316</v>
@@ -5180,7 +5189,7 @@
         <v>318</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="AB4" s="3" t="s">
         <v>319</v>
@@ -5276,16 +5285,16 @@
     </row>
     <row r="6" spans="1:42" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>622</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>616</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>624</v>
       </c>
       <c r="E6" s="9">
         <v>9606</v>
@@ -5327,13 +5336,13 @@
         <v>333</v>
       </c>
       <c r="R6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="S6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="T6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="U6" s="7" t="s">
         <v>335</v>
@@ -5342,7 +5351,7 @@
         <v>336</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>
@@ -5355,7 +5364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AG6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4:H4"/>
     </sheetView>
   </sheetViews>
@@ -5548,7 +5557,7 @@
         <v>372</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>373</v>
@@ -5632,10 +5641,10 @@
         <v>391</v>
       </c>
       <c r="G4" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H4" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>392</v>
@@ -5701,7 +5710,7 @@
         <v>372</v>
       </c>
       <c r="AD4" s="3" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="AE4" s="3" t="s">
         <v>404</v>
@@ -5749,16 +5758,16 @@
     </row>
     <row r="6" spans="1:33" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>625</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>622</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>627</v>
       </c>
       <c r="E6" s="6">
         <v>9606</v>
@@ -5827,10 +5836,10 @@
         <v>10000</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="AF6" s="7" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -5883,7 +5892,7 @@
         <v>415</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>351</v>
@@ -5918,7 +5927,7 @@
         <v>422</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>373</v>
@@ -5972,7 +5981,7 @@
         <v>434</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>435</v>
@@ -6001,16 +6010,16 @@
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>424</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>438</v>
@@ -6025,10 +6034,10 @@
         <v>428</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>439</v>
@@ -6036,16 +6045,16 @@
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>424</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>440</v>
@@ -6060,10 +6069,10 @@
         <v>428</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>439</v>
@@ -6071,16 +6080,16 @@
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>424</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>441</v>
@@ -6095,10 +6104,10 @@
         <v>428</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>439</v>
@@ -6269,31 +6278,31 @@
         <v>463</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>669</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>671</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>672</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>673</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -6318,13 +6327,13 @@
     </row>
     <row r="6" spans="1:16" s="7" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>628</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>630</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>456</v>
@@ -6468,13 +6477,13 @@
         <v>584</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>675</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -6492,13 +6501,13 @@
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>631</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>632</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>633</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>456</v>
@@ -6529,8 +6538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6655,23 +6664,23 @@
       <c r="F4" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>591</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>592</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>696</v>
+      </c>
+      <c r="H4" t="s">
+        <v>697</v>
+      </c>
+      <c r="I4" t="s">
+        <v>698</v>
+      </c>
+      <c r="J4" t="s">
         <v>604</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>605</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>606</v>
+      <c r="K4" t="s">
+        <v>699</v>
+      </c>
+      <c r="L4" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -6693,13 +6702,13 @@
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>640</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>641</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>642</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>456</v>

</xml_diff>